<commit_message>
Added DAC80508 test file
</commit_message>
<xml_diff>
--- a/Registers.xlsx
+++ b/Registers.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7b0877819b81e9be/Documents/Research Internship/Programs/xem7310_starter/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7b0877819b81e9be/Documents/Research Internship/Programs/covg_fpga/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="219" documentId="8_{A16721ED-633F-4336-9715-99B32CEC4535}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CC14F220-197C-4646-AD13-9358C010A540}"/>
+  <xr:revisionPtr revIDLastSave="261" documentId="8_{A16721ED-633F-4336-9715-99B32CEC4535}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EC4771FE-0F41-4FDB-9C9F-36B219595497}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="2" activeTab="5" xr2:uid="{C3AB243F-651F-4CB0-B6E1-3CA4785EC4D9}"/>
+    <workbookView xWindow="-6600" yWindow="1580" windowWidth="14400" windowHeight="7360" firstSheet="5" activeTab="5" xr2:uid="{C3AB243F-651F-4CB0-B6E1-3CA4785EC4D9}"/>
   </bookViews>
   <sheets>
     <sheet name="I2C" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="SPI_WB_1" sheetId="4" r:id="rId4"/>
     <sheet name="SPI_WB_2" sheetId="5" r:id="rId5"/>
     <sheet name="DAC80508" sheetId="6" r:id="rId6"/>
+    <sheet name="DAC80508_CONFIG" sheetId="7" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">I2C!$A$1:$E$6</definedName>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="97">
   <si>
     <t>Name</t>
   </si>
@@ -200,15 +201,9 @@
     <t>NOP</t>
   </si>
   <si>
-    <t>DEVICE ID</t>
-  </si>
-  <si>
     <t>SYNC</t>
   </si>
   <si>
-    <t>CONFI</t>
-  </si>
-  <si>
     <t>GAIN</t>
   </si>
   <si>
@@ -288,6 +283,57 @@
   </si>
   <si>
     <t>0xff00</t>
+  </si>
+  <si>
+    <t>CONFIG</t>
+  </si>
+  <si>
+    <t>ALM-SEL</t>
+  </si>
+  <si>
+    <t>ALM-EN</t>
+  </si>
+  <si>
+    <t>CRC-EN</t>
+  </si>
+  <si>
+    <t>FSDO</t>
+  </si>
+  <si>
+    <t>DSDO</t>
+  </si>
+  <si>
+    <t>REF-PWDWN</t>
+  </si>
+  <si>
+    <t>DAC7-PWDWN</t>
+  </si>
+  <si>
+    <t>DAC6-PWDWN</t>
+  </si>
+  <si>
+    <t>DAC5-PWDWN</t>
+  </si>
+  <si>
+    <t>DAC4-PWDWN</t>
+  </si>
+  <si>
+    <t>DAC3-PWDWN</t>
+  </si>
+  <si>
+    <t>DAC2-PWDWN</t>
+  </si>
+  <si>
+    <t>DAC1-PWDWN</t>
+  </si>
+  <si>
+    <t>DAC0-PWDWN</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>0x0896</t>
   </si>
 </sst>
 </file>
@@ -1308,12 +1354,12 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.7265625" customWidth="1"/>
+    <col min="1" max="1" width="14.08984375" customWidth="1"/>
     <col min="2" max="2" width="15.08984375" customWidth="1"/>
     <col min="3" max="3" width="16.26953125" customWidth="1"/>
   </cols>
@@ -1354,13 +1400,13 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>95</v>
       </c>
       <c r="B3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>46</v>
+        <v>96</v>
       </c>
       <c r="D3">
         <v>16</v>
@@ -1371,13 +1417,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D4">
         <v>16</v>
@@ -1388,10 +1434,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>54</v>
+        <v>80</v>
       </c>
       <c r="B5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C5" t="s">
         <v>46</v>
@@ -1405,10 +1451,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C6" t="s">
         <v>46</v>
@@ -1425,7 +1471,7 @@
         <v>37</v>
       </c>
       <c r="B7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C7" t="s">
         <v>46</v>
@@ -1439,10 +1485,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C8" t="s">
         <v>46</v>
@@ -1456,10 +1502,10 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B9" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C9" t="s">
         <v>46</v>
@@ -1473,10 +1519,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C10" t="s">
         <v>46</v>
@@ -1490,10 +1536,10 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C11" t="s">
         <v>46</v>
@@ -1507,10 +1553,10 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B12" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C12" t="s">
         <v>46</v>
@@ -1524,10 +1570,10 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B13" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C13" t="s">
         <v>46</v>
@@ -1541,10 +1587,10 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B14" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C14" t="s">
         <v>46</v>
@@ -1558,10 +1604,10 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B15" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C15" t="s">
         <v>46</v>
@@ -1575,10 +1621,10 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B16" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C16" t="s">
         <v>46</v>
@@ -1592,10 +1638,10 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B17" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C17" t="s">
         <v>46</v>
@@ -1611,4 +1657,279 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD157825-FA55-4A1C-B340-312146B82B8E}">
+  <dimension ref="A1:E15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="13.90625" customWidth="1"/>
+    <col min="2" max="2" width="12.6328125" customWidth="1"/>
+    <col min="3" max="3" width="14.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>86</v>
+      </c>
+      <c r="B7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>87</v>
+      </c>
+      <c r="B8" t="s">
+        <v>66</v>
+      </c>
+      <c r="C8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>88</v>
+      </c>
+      <c r="B9" t="s">
+        <v>66</v>
+      </c>
+      <c r="C9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>89</v>
+      </c>
+      <c r="B10" t="s">
+        <v>66</v>
+      </c>
+      <c r="C10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>90</v>
+      </c>
+      <c r="B11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C11" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>91</v>
+      </c>
+      <c r="B12" t="s">
+        <v>66</v>
+      </c>
+      <c r="C12" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>92</v>
+      </c>
+      <c r="B13" t="s">
+        <v>66</v>
+      </c>
+      <c r="C13" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>93</v>
+      </c>
+      <c r="B14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C14" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>94</v>
+      </c>
+      <c r="B15" t="s">
+        <v>66</v>
+      </c>
+      <c r="C15" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed DAC python errors before FPGA connection
</commit_message>
<xml_diff>
--- a/Registers.xlsx
+++ b/Registers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7b0877819b81e9be/Documents/Research Internship/Programs/covg_fpga/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="261" documentId="8_{A16721ED-633F-4336-9715-99B32CEC4535}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EC4771FE-0F41-4FDB-9C9F-36B219595497}"/>
+  <xr:revisionPtr revIDLastSave="314" documentId="8_{A16721ED-633F-4336-9715-99B32CEC4535}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B8E3633E-9524-4765-B589-78F5AFF7335F}"/>
   <bookViews>
-    <workbookView xWindow="-6600" yWindow="1580" windowWidth="14400" windowHeight="7360" firstSheet="5" activeTab="5" xr2:uid="{C3AB243F-651F-4CB0-B6E1-3CA4785EC4D9}"/>
+    <workbookView xWindow="0" yWindow="1580" windowWidth="14400" windowHeight="7360" firstSheet="2" activeTab="4" xr2:uid="{C3AB243F-651F-4CB0-B6E1-3CA4785EC4D9}"/>
   </bookViews>
   <sheets>
     <sheet name="I2C" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="97">
   <si>
     <t>Name</t>
   </si>
@@ -57,9 +57,6 @@
     <t>Bit Width</t>
   </si>
   <si>
-    <t>Bit Index</t>
-  </si>
-  <si>
     <t>0x40</t>
   </si>
   <si>
@@ -84,12 +81,6 @@
     <t>0x0000ffff</t>
   </si>
   <si>
-    <t>[15:0]</t>
-  </si>
-  <si>
-    <t>[7:0]</t>
-  </si>
-  <si>
     <t>0xffff</t>
   </si>
   <si>
@@ -334,6 +325,15 @@
   </si>
   <si>
     <t>0x0896</t>
+  </si>
+  <si>
+    <t>Bit Index (High)</t>
+  </si>
+  <si>
+    <t>Bit Index (Low)</t>
+  </si>
+  <si>
+    <t>TRIGGER_BIT</t>
   </si>
 </sst>
 </file>
@@ -390,8 +390,8 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -707,10 +707,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{235290A7-75FE-4F10-817B-094022AE6900}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -718,9 +718,11 @@
     <col min="1" max="1" width="22.453125" customWidth="1"/>
     <col min="2" max="2" width="13.08984375" customWidth="1"/>
     <col min="3" max="3" width="13.7265625" customWidth="1"/>
+    <col min="5" max="5" width="14" customWidth="1"/>
+    <col min="6" max="6" width="13.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -734,18 +736,21 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>94</v>
+      </c>
+      <c r="F1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
       <c r="C2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -753,16 +758,19 @@
       <c r="E2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -770,57 +778,75 @@
       <c r="E3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D4">
         <v>8</v>
       </c>
       <c r="E4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D5">
         <v>16</v>
       </c>
       <c r="E5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+      <c r="F5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D6">
         <v>16</v>
       </c>
       <c r="E6" t="s">
-        <v>10</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="F6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F12" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -829,18 +855,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D5E5B8F-5BB7-4168-B07F-5847C1B5455F}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="19.36328125" customWidth="1"/>
+    <col min="5" max="5" width="13.6328125" customWidth="1"/>
+    <col min="6" max="6" width="14.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -854,58 +882,70 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+        <v>94</v>
+      </c>
+      <c r="F1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
         <v>21</v>
       </c>
-      <c r="B2" t="s">
-        <v>24</v>
-      </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D2">
         <v>16</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
         <v>22</v>
       </c>
-      <c r="B3" t="s">
-        <v>25</v>
-      </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D3">
         <v>16</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D4">
         <v>16</v>
       </c>
       <c r="E4" t="s">
-        <v>10</v>
+        <v>9</v>
+      </c>
+      <c r="F4" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -915,10 +955,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AF12F6B-39D7-464E-AFAC-DA98604DB1A5}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -926,9 +966,11 @@
     <col min="1" max="1" width="18.6328125" customWidth="1"/>
     <col min="2" max="2" width="13.36328125" customWidth="1"/>
     <col min="3" max="3" width="14.54296875" customWidth="1"/>
+    <col min="5" max="5" width="14.1796875" customWidth="1"/>
+    <col min="6" max="6" width="13.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -942,228 +984,270 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+        <v>94</v>
+      </c>
+      <c r="F1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D2">
         <v>32</v>
       </c>
       <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
       </c>
       <c r="D3">
         <v>32</v>
       </c>
       <c r="E3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
       </c>
       <c r="D4">
         <v>32</v>
       </c>
       <c r="E4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
       </c>
       <c r="D5">
         <v>32</v>
       </c>
       <c r="E5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" t="s">
-        <v>11</v>
       </c>
       <c r="D6">
         <v>32</v>
       </c>
       <c r="E6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7" t="s">
-        <v>38</v>
-      </c>
-      <c r="C7" t="s">
-        <v>11</v>
       </c>
       <c r="D7">
         <v>32</v>
       </c>
       <c r="E7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>31</v>
-      </c>
-      <c r="B8" t="s">
-        <v>39</v>
-      </c>
-      <c r="C8" t="s">
-        <v>11</v>
       </c>
       <c r="D8">
         <v>32</v>
       </c>
       <c r="E8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>32</v>
-      </c>
-      <c r="B9" t="s">
-        <v>40</v>
-      </c>
-      <c r="C9" t="s">
-        <v>11</v>
       </c>
       <c r="D9">
         <v>32</v>
       </c>
       <c r="E9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>33</v>
-      </c>
-      <c r="B10" t="s">
-        <v>41</v>
-      </c>
-      <c r="C10" t="s">
-        <v>11</v>
       </c>
       <c r="D10">
         <f>8*4</f>
         <v>32</v>
       </c>
       <c r="E10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+      <c r="F10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B11" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D11">
         <v>32</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E11" s="2">
+        <v>15</v>
+      </c>
+      <c r="F11" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D12">
         <v>32</v>
       </c>
-      <c r="E12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E12" s="2">
+        <v>7</v>
+      </c>
+      <c r="F12" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B13" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D13">
         <v>32</v>
       </c>
       <c r="E13" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+      <c r="F13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>37</v>
+        <v>96</v>
       </c>
       <c r="B14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C14" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D14">
         <v>1</v>
       </c>
       <c r="E14">
+        <v>3</v>
+      </c>
+      <c r="F14">
         <v>3</v>
       </c>
     </row>
@@ -1175,10 +1259,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B40B7BE3-9A42-42BA-88D6-9D009061040B}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1186,9 +1270,11 @@
     <col min="1" max="1" width="11.26953125" customWidth="1"/>
     <col min="2" max="2" width="13.90625" customWidth="1"/>
     <col min="3" max="3" width="15.54296875" customWidth="1"/>
+    <col min="5" max="5" width="14.1796875" customWidth="1"/>
+    <col min="6" max="6" width="13.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1202,57 +1288,69 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+        <v>94</v>
+      </c>
+      <c r="F1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D2">
         <v>32</v>
       </c>
       <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
       </c>
       <c r="D3">
         <v>32</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>96</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4">
+        <v>4</v>
+      </c>
+      <c r="F4">
         <v>4</v>
       </c>
     </row>
@@ -1263,10 +1361,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE81132C-CE5C-48CD-A64A-B3A385985B9A}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1274,9 +1372,11 @@
     <col min="1" max="1" width="11.453125" customWidth="1"/>
     <col min="2" max="2" width="13.453125" customWidth="1"/>
     <col min="3" max="3" width="15.81640625" customWidth="1"/>
+    <col min="5" max="5" width="14.08984375" customWidth="1"/>
+    <col min="6" max="6" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1290,57 +1390,69 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+        <v>94</v>
+      </c>
+      <c r="F1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D2">
         <v>32</v>
       </c>
       <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
       </c>
       <c r="D3">
         <v>32</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>96</v>
       </c>
       <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
         <v>5</v>
       </c>
-      <c r="C4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
+      <c r="F4">
         <v>5</v>
       </c>
     </row>
@@ -1351,10 +1463,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C9C2D46-1736-43E0-82AF-3E209A55AC59}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1362,9 +1474,11 @@
     <col min="1" max="1" width="14.08984375" customWidth="1"/>
     <col min="2" max="2" width="15.08984375" customWidth="1"/>
     <col min="3" max="3" width="16.26953125" customWidth="1"/>
+    <col min="5" max="5" width="14.6328125" customWidth="1"/>
+    <col min="6" max="6" width="14.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1378,279 +1492,330 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+        <v>94</v>
+      </c>
+      <c r="F1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D2">
         <v>16</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>96</v>
+        <v>61</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>93</v>
       </c>
       <c r="D3">
         <v>16</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D4">
         <v>16</v>
       </c>
       <c r="E4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D5">
         <v>16</v>
       </c>
       <c r="E5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+      <c r="F5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B6" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D6">
         <v>16</v>
       </c>
       <c r="E6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+      <c r="F6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D7">
         <v>16</v>
       </c>
       <c r="E7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+      <c r="F7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B8" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C8" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D8">
         <v>16</v>
       </c>
       <c r="E8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+      <c r="F8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B9" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C9" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D9">
         <v>16</v>
       </c>
       <c r="E9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+      <c r="F9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B10" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C10" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D10">
         <v>16</v>
       </c>
       <c r="E10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+      <c r="F10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C11" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D11">
         <v>16</v>
       </c>
       <c r="E11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+      <c r="F11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B12" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C12" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D12">
         <v>16</v>
       </c>
       <c r="E12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+      <c r="F12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B13" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C13" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D13">
         <v>16</v>
       </c>
       <c r="E13" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+      <c r="F13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B14" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C14" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D14">
         <v>16</v>
       </c>
       <c r="E14" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+      <c r="F14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B15" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C15" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D15">
         <v>16</v>
       </c>
       <c r="E15" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+      <c r="F15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B16" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C16" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D16">
         <v>16</v>
       </c>
       <c r="E16" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+      <c r="F16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B17" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C17" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D17">
         <v>16</v>
       </c>
       <c r="E17" t="s">
-        <v>10</v>
+        <v>9</v>
+      </c>
+      <c r="F17" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -1661,10 +1826,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD157825-FA55-4A1C-B340-312146B82B8E}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E1"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1672,9 +1837,11 @@
     <col min="1" max="1" width="13.90625" customWidth="1"/>
     <col min="2" max="2" width="12.6328125" customWidth="1"/>
     <col min="3" max="3" width="14.6328125" customWidth="1"/>
+    <col min="5" max="5" width="15.1796875" customWidth="1"/>
+    <col min="6" max="6" width="14.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1688,18 +1855,21 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+        <v>94</v>
+      </c>
+      <c r="F1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -1707,16 +1877,19 @@
       <c r="E2">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -1724,16 +1897,19 @@
       <c r="E3">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -1741,16 +1917,19 @@
       <c r="E4">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F4">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -1758,16 +1937,19 @@
       <c r="E5">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -1775,16 +1957,19 @@
       <c r="E6">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B7" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C7" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -1792,16 +1977,19 @@
       <c r="E7">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C8" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -1809,16 +1997,19 @@
       <c r="E8">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B9" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C9" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -1826,16 +2017,19 @@
       <c r="E9">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B10" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C10" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -1843,16 +2037,19 @@
       <c r="E10">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B11" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C11" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -1860,16 +2057,19 @@
       <c r="E11">
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B12" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C12" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -1877,16 +2077,19 @@
       <c r="E12">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B13" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C13" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -1894,16 +2097,19 @@
       <c r="E13">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B14" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C14" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -1911,21 +2117,27 @@
       <c r="E14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B15" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C15" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D15">
         <v>1</v>
       </c>
       <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added OK endpoints for DAC Wishbones
</commit_message>
<xml_diff>
--- a/Registers.xlsx
+++ b/Registers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7b0877819b81e9be/Documents/Research Internship/Programs/covg_fpga/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="402" documentId="8_{A16721ED-633F-4336-9715-99B32CEC4535}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{86F059E9-E16E-4147-94E2-694E4C270C9B}"/>
+  <xr:revisionPtr revIDLastSave="420" documentId="8_{A16721ED-633F-4336-9715-99B32CEC4535}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F66DA180-530D-496B-8A24-06A4BA235B96}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="2" activeTab="7" xr2:uid="{C3AB243F-651F-4CB0-B6E1-3CA4785EC4D9}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="2" activeTab="5" xr2:uid="{C3AB243F-651F-4CB0-B6E1-3CA4785EC4D9}"/>
   </bookViews>
   <sheets>
     <sheet name="I2C" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="117">
   <si>
     <t>Name</t>
   </si>
@@ -383,6 +383,18 @@
   </si>
   <si>
     <t>0x03</t>
+  </si>
+  <si>
+    <t>WB_IN_1</t>
+  </si>
+  <si>
+    <t>WB_IN_0</t>
+  </si>
+  <si>
+    <t>WB_OUT_0</t>
+  </si>
+  <si>
+    <t>WB_OUT_1</t>
   </si>
 </sst>
 </file>
@@ -1497,10 +1509,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C9C2D46-1736-43E0-82AF-3E209A55AC59}">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1849,6 +1861,86 @@
         <v>9</v>
       </c>
       <c r="F17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>114</v>
+      </c>
+      <c r="B18" t="s">
+        <v>112</v>
+      </c>
+      <c r="C18" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18">
+        <v>32</v>
+      </c>
+      <c r="E18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>113</v>
+      </c>
+      <c r="B19" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19">
+        <v>32</v>
+      </c>
+      <c r="E19" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>115</v>
+      </c>
+      <c r="B20" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20">
+        <v>32</v>
+      </c>
+      <c r="E20" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>116</v>
+      </c>
+      <c r="B21" t="s">
+        <v>47</v>
+      </c>
+      <c r="C21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21">
+        <v>32</v>
+      </c>
+      <c r="E21" t="s">
+        <v>9</v>
+      </c>
+      <c r="F21" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2184,7 +2276,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDACA481-2925-4EA7-BD1F-BDE6CBFB0E5A}">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added methods to ID chip class
</commit_message>
<xml_diff>
--- a/Registers.xlsx
+++ b/Registers.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7b0877819b81e9be/Documents/Research Internship/Programs/covg_fpga/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="432" documentId="8_{A16721ED-633F-4336-9715-99B32CEC4535}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EAF08BA3-B769-4C12-AC19-3759B0906965}"/>
+  <xr:revisionPtr revIDLastSave="465" documentId="8_{A16721ED-633F-4336-9715-99B32CEC4535}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3D36EF1E-75C1-4675-97CE-A4BADAE71B76}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="2" activeTab="2" xr2:uid="{C3AB243F-651F-4CB0-B6E1-3CA4785EC4D9}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{C3AB243F-651F-4CB0-B6E1-3CA4785EC4D9}"/>
   </bookViews>
   <sheets>
     <sheet name="I2C" sheetId="1" r:id="rId1"/>
     <sheet name="IOExpander" sheetId="3" r:id="rId2"/>
-    <sheet name="SPI" sheetId="2" r:id="rId3"/>
-    <sheet name="SPI_WB_1" sheetId="4" r:id="rId4"/>
-    <sheet name="SPI_WB_2" sheetId="5" r:id="rId5"/>
-    <sheet name="DAC80508" sheetId="6" r:id="rId6"/>
-    <sheet name="DAC80508_CONFIG" sheetId="7" r:id="rId7"/>
-    <sheet name="clamp_configuration" sheetId="8" r:id="rId8"/>
+    <sheet name="24AA025UID" sheetId="9" r:id="rId3"/>
+    <sheet name="SPI" sheetId="2" r:id="rId4"/>
+    <sheet name="SPI_WB_1" sheetId="4" r:id="rId5"/>
+    <sheet name="SPI_WB_2" sheetId="5" r:id="rId6"/>
+    <sheet name="DAC80508" sheetId="6" r:id="rId7"/>
+    <sheet name="DAC80508_CONFIG" sheetId="7" r:id="rId8"/>
+    <sheet name="clamp_configuration" sheetId="8" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">I2C!$A$1:$E$6</definedName>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="127">
   <si>
     <t>Name</t>
   </si>
@@ -401,13 +402,37 @@
   </si>
   <si>
     <t>DIVIDER</t>
+  </si>
+  <si>
+    <t>SERIAL_NUMBER</t>
+  </si>
+  <si>
+    <t>MANUFACTURER_CODE</t>
+  </si>
+  <si>
+    <t>DEVICE_CODE</t>
+  </si>
+  <si>
+    <t>0x29</t>
+  </si>
+  <si>
+    <t>0x41</t>
+  </si>
+  <si>
+    <t>0xfc</t>
+  </si>
+  <si>
+    <t>0xfa</t>
+  </si>
+  <si>
+    <t>0xfb</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -421,13 +446,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -439,14 +476,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -910,7 +950,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1006,10 +1046,112 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA3DCDAD-A104-45B0-9B4C-29AE8EC77D31}">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="21.7265625" customWidth="1"/>
+    <col min="2" max="2" width="14.26953125" customWidth="1"/>
+    <col min="3" max="3" width="16.90625" customWidth="1"/>
+    <col min="5" max="5" width="16" customWidth="1"/>
+    <col min="6" max="6" width="15.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2">
+        <v>32</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B3" t="s">
+        <v>125</v>
+      </c>
+      <c r="C3" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>121</v>
+      </c>
+      <c r="B4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C4" t="s">
+        <v>123</v>
+      </c>
+      <c r="D4">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AF12F6B-39D7-464E-AFAC-DA98604DB1A5}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
@@ -1309,7 +1451,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B40B7BE3-9A42-42BA-88D6-9D009061040B}">
   <dimension ref="A1:F4"/>
   <sheetViews>
@@ -1411,7 +1553,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE81132C-CE5C-48CD-A64A-B3A385985B9A}">
   <dimension ref="A1:F4"/>
   <sheetViews>
@@ -1513,7 +1655,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C9C2D46-1736-43E0-82AF-3E209A55AC59}">
   <dimension ref="A1:F23"/>
   <sheetViews>
@@ -1996,7 +2138,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD157825-FA55-4A1C-B340-312146B82B8E}">
   <dimension ref="A1:F15"/>
   <sheetViews>
@@ -2318,7 +2460,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDACA481-2925-4EA7-BD1F-BDE6CBFB0E5A}">
   <dimension ref="A1:F16"/>
   <sheetViews>

</xml_diff>

<commit_message>
Change from parameters to registers and endpoints
</commit_message>
<xml_diff>
--- a/Registers.xlsx
+++ b/Registers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7b0877819b81e9be/Documents/Research Internship/Programs/covg_fpga/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="29" documentId="13_ncr:1_{F648551C-414A-4D29-BD04-FC429653B53D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{77A2F53B-3CE1-46E2-A32E-9197F4EB24EB}"/>
+  <xr:revisionPtr revIDLastSave="33" documentId="13_ncr:1_{F648551C-414A-4D29-BD04-FC429653B53D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5C27BAC6-34B1-4CA1-8B62-F207474C8104}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{C3AB243F-651F-4CB0-B6E1-3CA4785EC4D9}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="5" activeTab="10" xr2:uid="{C3AB243F-651F-4CB0-B6E1-3CA4785EC4D9}"/>
   </bookViews>
   <sheets>
     <sheet name="I2C" sheetId="1" r:id="rId1"/>
@@ -23,11 +23,10 @@
     <sheet name="SPI_WB_1" sheetId="4" r:id="rId8"/>
     <sheet name="SPI_WB_2" sheetId="5" r:id="rId9"/>
     <sheet name="DAC80508" sheetId="6" r:id="rId10"/>
-    <sheet name="DAC80508_CONFIG" sheetId="7" r:id="rId11"/>
-    <sheet name="AD5453" sheetId="14" r:id="rId12"/>
-    <sheet name="ADS7952" sheetId="15" r:id="rId13"/>
-    <sheet name="ADS8686" sheetId="16" r:id="rId14"/>
-    <sheet name="AD7961" sheetId="13" r:id="rId15"/>
+    <sheet name="AD5453" sheetId="14" r:id="rId11"/>
+    <sheet name="ADS7952" sheetId="15" r:id="rId12"/>
+    <sheet name="ADS8686" sheetId="16" r:id="rId13"/>
+    <sheet name="AD7961" sheetId="13" r:id="rId14"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">I2C!$A$1:$E$6</definedName>
@@ -52,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="201">
   <si>
     <t>Name</t>
   </si>
@@ -1191,10 +1190,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C9C2D46-1736-43E0-82AF-3E209A55AC59}">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1548,90 +1547,90 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>109</v>
+        <v>73</v>
       </c>
       <c r="B18" t="s">
-        <v>107</v>
+        <v>58</v>
       </c>
       <c r="C18" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
       <c r="D18">
-        <v>32</v>
-      </c>
-      <c r="E18" t="s">
-        <v>9</v>
-      </c>
-      <c r="F18" t="s">
-        <v>9</v>
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>13</v>
+      </c>
+      <c r="F18">
+        <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>108</v>
+        <v>74</v>
       </c>
       <c r="B19" t="s">
-        <v>30</v>
+        <v>58</v>
       </c>
       <c r="C19" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
       <c r="D19">
-        <v>32</v>
-      </c>
-      <c r="E19" t="s">
-        <v>9</v>
-      </c>
-      <c r="F19" t="s">
-        <v>9</v>
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>12</v>
+      </c>
+      <c r="F19">
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>110</v>
+        <v>75</v>
       </c>
       <c r="B20" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="C20" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
       <c r="D20">
-        <v>32</v>
-      </c>
-      <c r="E20" t="s">
-        <v>9</v>
-      </c>
-      <c r="F20" t="s">
-        <v>9</v>
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>11</v>
+      </c>
+      <c r="F20">
+        <v>11</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>111</v>
+        <v>76</v>
       </c>
       <c r="B21" t="s">
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="C21" t="s">
+        <v>37</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21">
         <v>10</v>
       </c>
-      <c r="D21">
-        <v>32</v>
-      </c>
-      <c r="E21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F21" t="s">
-        <v>9</v>
+      <c r="F21">
+        <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>113</v>
+        <v>77</v>
       </c>
       <c r="B22" t="s">
-        <v>4</v>
+        <v>58</v>
       </c>
       <c r="C22" t="s">
         <v>37</v>
@@ -1640,29 +1639,309 @@
         <v>1</v>
       </c>
       <c r="E22">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F22">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
+        <v>78</v>
+      </c>
+      <c r="B23" t="s">
+        <v>58</v>
+      </c>
+      <c r="C23" t="s">
+        <v>37</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>8</v>
+      </c>
+      <c r="F23">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>79</v>
+      </c>
+      <c r="B24" t="s">
+        <v>58</v>
+      </c>
+      <c r="C24" t="s">
+        <v>37</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>7</v>
+      </c>
+      <c r="F24">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>80</v>
+      </c>
+      <c r="B25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C25" t="s">
+        <v>37</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <v>6</v>
+      </c>
+      <c r="F25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>81</v>
+      </c>
+      <c r="B26" t="s">
+        <v>58</v>
+      </c>
+      <c r="C26" t="s">
+        <v>37</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <v>5</v>
+      </c>
+      <c r="F26">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>82</v>
+      </c>
+      <c r="B27" t="s">
+        <v>58</v>
+      </c>
+      <c r="C27" t="s">
+        <v>37</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>4</v>
+      </c>
+      <c r="F27">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>83</v>
+      </c>
+      <c r="B28" t="s">
+        <v>58</v>
+      </c>
+      <c r="C28" t="s">
+        <v>37</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28">
+        <v>3</v>
+      </c>
+      <c r="F28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>84</v>
+      </c>
+      <c r="B29" t="s">
+        <v>58</v>
+      </c>
+      <c r="C29" t="s">
+        <v>37</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <v>2</v>
+      </c>
+      <c r="F29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>85</v>
+      </c>
+      <c r="B30" t="s">
+        <v>58</v>
+      </c>
+      <c r="C30" t="s">
+        <v>37</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+      <c r="F30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>86</v>
+      </c>
+      <c r="B31" t="s">
+        <v>58</v>
+      </c>
+      <c r="C31" t="s">
+        <v>37</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>109</v>
+      </c>
+      <c r="B32" t="s">
+        <v>107</v>
+      </c>
+      <c r="C32" t="s">
+        <v>10</v>
+      </c>
+      <c r="D32">
+        <v>32</v>
+      </c>
+      <c r="E32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F32" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>108</v>
+      </c>
+      <c r="B33" t="s">
+        <v>30</v>
+      </c>
+      <c r="C33" t="s">
+        <v>10</v>
+      </c>
+      <c r="D33">
+        <v>32</v>
+      </c>
+      <c r="E33" t="s">
+        <v>9</v>
+      </c>
+      <c r="F33" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>110</v>
+      </c>
+      <c r="B34" t="s">
+        <v>40</v>
+      </c>
+      <c r="C34" t="s">
+        <v>10</v>
+      </c>
+      <c r="D34">
+        <v>32</v>
+      </c>
+      <c r="E34" t="s">
+        <v>9</v>
+      </c>
+      <c r="F34" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>111</v>
+      </c>
+      <c r="B35" t="s">
+        <v>42</v>
+      </c>
+      <c r="C35" t="s">
+        <v>10</v>
+      </c>
+      <c r="D35">
+        <v>32</v>
+      </c>
+      <c r="E35" t="s">
+        <v>9</v>
+      </c>
+      <c r="F35" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>113</v>
+      </c>
+      <c r="B36" t="s">
+        <v>4</v>
+      </c>
+      <c r="C36" t="s">
+        <v>37</v>
+      </c>
+      <c r="D36">
+        <v>1</v>
+      </c>
+      <c r="E36">
+        <v>8</v>
+      </c>
+      <c r="F36">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
         <v>112</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B37" t="s">
         <v>4</v>
       </c>
-      <c r="C23" t="s">
-        <v>37</v>
-      </c>
-      <c r="D23">
-        <v>1</v>
-      </c>
-      <c r="E23">
-        <v>9</v>
-      </c>
-      <c r="F23">
+      <c r="C37" t="s">
+        <v>37</v>
+      </c>
+      <c r="D37">
+        <v>1</v>
+      </c>
+      <c r="E37">
+        <v>9</v>
+      </c>
+      <c r="F37">
         <v>9</v>
       </c>
     </row>
@@ -1673,332 +1952,10 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD157825-FA55-4A1C-B340-312146B82B8E}">
-  <dimension ref="A1:F15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="13.81640625" customWidth="1"/>
-    <col min="2" max="2" width="12.453125" customWidth="1"/>
-    <col min="3" max="3" width="14.453125" customWidth="1"/>
-    <col min="5" max="5" width="15.1796875" customWidth="1"/>
-    <col min="6" max="6" width="14.81640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>88</v>
-      </c>
-      <c r="F1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>13</v>
-      </c>
-      <c r="F2">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>12</v>
-      </c>
-      <c r="F3">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>75</v>
-      </c>
-      <c r="B4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>11</v>
-      </c>
-      <c r="F4">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>76</v>
-      </c>
-      <c r="B5" t="s">
-        <v>58</v>
-      </c>
-      <c r="C5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5">
-        <v>10</v>
-      </c>
-      <c r="F5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>77</v>
-      </c>
-      <c r="B6" t="s">
-        <v>58</v>
-      </c>
-      <c r="C6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6">
-        <v>9</v>
-      </c>
-      <c r="F6">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>78</v>
-      </c>
-      <c r="B7" t="s">
-        <v>58</v>
-      </c>
-      <c r="C7" t="s">
-        <v>37</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7">
-        <v>8</v>
-      </c>
-      <c r="F7">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>79</v>
-      </c>
-      <c r="B8" t="s">
-        <v>58</v>
-      </c>
-      <c r="C8" t="s">
-        <v>37</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="E8">
-        <v>7</v>
-      </c>
-      <c r="F8">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>80</v>
-      </c>
-      <c r="B9" t="s">
-        <v>58</v>
-      </c>
-      <c r="C9" t="s">
-        <v>37</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9">
-        <v>6</v>
-      </c>
-      <c r="F9">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>81</v>
-      </c>
-      <c r="B10" t="s">
-        <v>58</v>
-      </c>
-      <c r="C10" t="s">
-        <v>37</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-      <c r="E10">
-        <v>5</v>
-      </c>
-      <c r="F10">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>82</v>
-      </c>
-      <c r="B11" t="s">
-        <v>58</v>
-      </c>
-      <c r="C11" t="s">
-        <v>37</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-      <c r="E11">
-        <v>4</v>
-      </c>
-      <c r="F11">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>83</v>
-      </c>
-      <c r="B12" t="s">
-        <v>58</v>
-      </c>
-      <c r="C12" t="s">
-        <v>37</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-      <c r="E12">
-        <v>3</v>
-      </c>
-      <c r="F12">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>84</v>
-      </c>
-      <c r="B13" t="s">
-        <v>58</v>
-      </c>
-      <c r="C13" t="s">
-        <v>37</v>
-      </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
-      <c r="E13">
-        <v>2</v>
-      </c>
-      <c r="F13">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>85</v>
-      </c>
-      <c r="B14" t="s">
-        <v>58</v>
-      </c>
-      <c r="C14" t="s">
-        <v>37</v>
-      </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
-      <c r="E14">
-        <v>1</v>
-      </c>
-      <c r="F14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>86</v>
-      </c>
-      <c r="B15" t="s">
-        <v>58</v>
-      </c>
-      <c r="C15" t="s">
-        <v>37</v>
-      </c>
-      <c r="D15">
-        <v>1</v>
-      </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-      <c r="F15">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{427C2A19-8BF7-4B8D-9492-08A4DEB2EF8C}">
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -2029,7 +1986,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9F9F601-34D5-480B-81CE-67CE1CDB2EB8}">
   <dimension ref="A1:F1"/>
   <sheetViews>
@@ -2064,7 +2021,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1CC0846-B885-4A4F-9321-B09606FEAD42}">
   <dimension ref="A1:F1"/>
   <sheetViews>
@@ -2099,7 +2056,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62F8966C-0492-4738-84AA-AA5E0C7A41BB}">
   <dimension ref="A1:F13"/>
   <sheetViews>
@@ -2535,7 +2492,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D5E5B8F-5BB7-4168-B07F-5847C1B5455F}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added ADS8686 registers to Registers.xlsx
</commit_message>
<xml_diff>
--- a/Registers.xlsx
+++ b/Registers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7b0877819b81e9be/Documents/Research Internship/Programs/covg_fpga/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/koer2434/Google Drive/UST/research/covg/fpga_and_measurements/daq_v2/covg_fpga/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="33" documentId="13_ncr:1_{F648551C-414A-4D29-BD04-FC429653B53D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5C27BAC6-34B1-4CA1-8B62-F207474C8104}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D93E9DF7-F579-BB40-A42C-03166C011540}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="5" activeTab="10" xr2:uid="{C3AB243F-651F-4CB0-B6E1-3CA4785EC4D9}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="22680" windowHeight="19860" firstSheet="5" activeTab="12" xr2:uid="{C3AB243F-651F-4CB0-B6E1-3CA4785EC4D9}"/>
   </bookViews>
   <sheets>
     <sheet name="I2C" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="706" uniqueCount="278">
   <si>
     <t>Name</t>
   </si>
@@ -654,6 +654,237 @@
   </si>
   <si>
     <t>adc_pll_lock</t>
+  </si>
+  <si>
+    <t>config</t>
+  </si>
+  <si>
+    <t>chan_sel</t>
+  </si>
+  <si>
+    <t>rangeA1</t>
+  </si>
+  <si>
+    <t>0xFF</t>
+  </si>
+  <si>
+    <t>rangeA2</t>
+  </si>
+  <si>
+    <t>rangeB1</t>
+  </si>
+  <si>
+    <t>rangeB2</t>
+  </si>
+  <si>
+    <t>0x07</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>over_rangeA</t>
+  </si>
+  <si>
+    <t>0xA</t>
+  </si>
+  <si>
+    <t>over_rangeB</t>
+  </si>
+  <si>
+    <t>0xB</t>
+  </si>
+  <si>
+    <t>lpf</t>
+  </si>
+  <si>
+    <t>0xC</t>
+  </si>
+  <si>
+    <t>devID</t>
+  </si>
+  <si>
+    <t>seq0</t>
+  </si>
+  <si>
+    <t>seq1</t>
+  </si>
+  <si>
+    <t>0x11</t>
+  </si>
+  <si>
+    <t>seq2</t>
+  </si>
+  <si>
+    <t>seq3</t>
+  </si>
+  <si>
+    <t>0x33</t>
+  </si>
+  <si>
+    <t>seq4</t>
+  </si>
+  <si>
+    <t>0x44</t>
+  </si>
+  <si>
+    <t>seq5</t>
+  </si>
+  <si>
+    <t>0x55</t>
+  </si>
+  <si>
+    <t>seq6</t>
+  </si>
+  <si>
+    <t>0x66</t>
+  </si>
+  <si>
+    <t>seq7</t>
+  </si>
+  <si>
+    <t>0x27</t>
+  </si>
+  <si>
+    <t>0x77</t>
+  </si>
+  <si>
+    <t>seq8</t>
+  </si>
+  <si>
+    <t>0x28</t>
+  </si>
+  <si>
+    <t>seq9</t>
+  </si>
+  <si>
+    <t>seq10</t>
+  </si>
+  <si>
+    <t>0x2A</t>
+  </si>
+  <si>
+    <t>seq11</t>
+  </si>
+  <si>
+    <t>0x2B</t>
+  </si>
+  <si>
+    <t>seq12</t>
+  </si>
+  <si>
+    <t>0x2C</t>
+  </si>
+  <si>
+    <t>seq13</t>
+  </si>
+  <si>
+    <t>0x2D</t>
+  </si>
+  <si>
+    <t>seq14</t>
+  </si>
+  <si>
+    <t>0x2E</t>
+  </si>
+  <si>
+    <t>seq15</t>
+  </si>
+  <si>
+    <t>0x2F</t>
+  </si>
+  <si>
+    <t>seq16</t>
+  </si>
+  <si>
+    <t>0x30</t>
+  </si>
+  <si>
+    <t>seq17</t>
+  </si>
+  <si>
+    <t>0x31</t>
+  </si>
+  <si>
+    <t>seq18</t>
+  </si>
+  <si>
+    <t>0x32</t>
+  </si>
+  <si>
+    <t>seq19</t>
+  </si>
+  <si>
+    <t>seq20</t>
+  </si>
+  <si>
+    <t>0x34</t>
+  </si>
+  <si>
+    <t>seq21</t>
+  </si>
+  <si>
+    <t>0x35</t>
+  </si>
+  <si>
+    <t>seq22</t>
+  </si>
+  <si>
+    <t>0x36</t>
+  </si>
+  <si>
+    <t>seq23</t>
+  </si>
+  <si>
+    <t>0x37</t>
+  </si>
+  <si>
+    <t>seq24</t>
+  </si>
+  <si>
+    <t>0x38</t>
+  </si>
+  <si>
+    <t>seq25</t>
+  </si>
+  <si>
+    <t>0x39</t>
+  </si>
+  <si>
+    <t>seq26</t>
+  </si>
+  <si>
+    <t>0x3A</t>
+  </si>
+  <si>
+    <t>seq27</t>
+  </si>
+  <si>
+    <t>0x3B</t>
+  </si>
+  <si>
+    <t>seq28</t>
+  </si>
+  <si>
+    <t>0x3C</t>
+  </si>
+  <si>
+    <t>seq29</t>
+  </si>
+  <si>
+    <t>0x3D</t>
+  </si>
+  <si>
+    <t>seq30</t>
+  </si>
+  <si>
+    <t>0x3E</t>
+  </si>
+  <si>
+    <t>seq31</t>
+  </si>
+  <si>
+    <t>0x3F</t>
   </si>
 </sst>
 </file>
@@ -1048,16 +1279,16 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.453125" customWidth="1"/>
-    <col min="2" max="2" width="13.1796875" customWidth="1"/>
-    <col min="3" max="3" width="13.54296875" customWidth="1"/>
+    <col min="1" max="1" width="22.5" customWidth="1"/>
+    <col min="2" max="2" width="13.1640625" customWidth="1"/>
+    <col min="3" max="3" width="13.5" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="13.1796875" customWidth="1"/>
+    <col min="6" max="6" width="13.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1077,7 +1308,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1097,7 +1328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -1117,7 +1348,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -1137,7 +1368,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -1157,7 +1388,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -1177,10 +1408,10 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F12" s="1"/>
     </row>
   </sheetData>
@@ -1196,16 +1427,16 @@
       <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.54296875" customWidth="1"/>
-    <col min="2" max="2" width="15.1796875" customWidth="1"/>
-    <col min="3" max="3" width="16.453125" customWidth="1"/>
-    <col min="5" max="5" width="14.453125" customWidth="1"/>
-    <col min="6" max="6" width="14.1796875" customWidth="1"/>
+    <col min="1" max="1" width="26.5" customWidth="1"/>
+    <col min="2" max="2" width="15.1640625" customWidth="1"/>
+    <col min="3" max="3" width="16.5" customWidth="1"/>
+    <col min="5" max="5" width="14.5" customWidth="1"/>
+    <col min="6" max="6" width="14.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1225,7 +1456,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>43</v>
       </c>
@@ -1245,7 +1476,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>87</v>
       </c>
@@ -1265,7 +1496,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>44</v>
       </c>
@@ -1285,7 +1516,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>72</v>
       </c>
@@ -1305,7 +1536,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>45</v>
       </c>
@@ -1325,7 +1556,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -1345,7 +1576,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>46</v>
       </c>
@@ -1365,7 +1596,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>47</v>
       </c>
@@ -1385,7 +1616,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>48</v>
       </c>
@@ -1405,7 +1636,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>49</v>
       </c>
@@ -1425,7 +1656,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>50</v>
       </c>
@@ -1445,7 +1676,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>51</v>
       </c>
@@ -1465,7 +1696,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>52</v>
       </c>
@@ -1485,7 +1716,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>53</v>
       </c>
@@ -1505,7 +1736,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>54</v>
       </c>
@@ -1525,7 +1756,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>55</v>
       </c>
@@ -1545,7 +1776,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>73</v>
       </c>
@@ -1565,7 +1796,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>74</v>
       </c>
@@ -1585,7 +1816,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>75</v>
       </c>
@@ -1605,7 +1836,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>76</v>
       </c>
@@ -1625,7 +1856,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>77</v>
       </c>
@@ -1645,7 +1876,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>78</v>
       </c>
@@ -1665,7 +1896,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>79</v>
       </c>
@@ -1685,7 +1916,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>80</v>
       </c>
@@ -1705,7 +1936,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>81</v>
       </c>
@@ -1725,7 +1956,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>82</v>
       </c>
@@ -1745,7 +1976,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>83</v>
       </c>
@@ -1765,7 +1996,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>84</v>
       </c>
@@ -1785,7 +2016,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>85</v>
       </c>
@@ -1805,7 +2036,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>86</v>
       </c>
@@ -1825,7 +2056,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>109</v>
       </c>
@@ -1845,7 +2076,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>108</v>
       </c>
@@ -1865,7 +2096,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>110</v>
       </c>
@@ -1885,7 +2116,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>111</v>
       </c>
@@ -1905,7 +2136,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>113</v>
       </c>
@@ -1925,7 +2156,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>112</v>
       </c>
@@ -1955,13 +2186,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{427C2A19-8BF7-4B8D-9492-08A4DEB2EF8C}">
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1994,9 +2225,9 @@
       <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2023,15 +2254,15 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1CC0846-B885-4A4F-9321-B09606FEAD42}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:F44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2049,6 +2280,866 @@
       </c>
       <c r="F1" t="s">
         <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>201</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>8</v>
+      </c>
+      <c r="E2">
+        <v>7</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>202</v>
+      </c>
+      <c r="B3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>8</v>
+      </c>
+      <c r="E3">
+        <v>7</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>203</v>
+      </c>
+      <c r="B4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" t="s">
+        <v>204</v>
+      </c>
+      <c r="D4">
+        <v>8</v>
+      </c>
+      <c r="E4">
+        <v>7</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>205</v>
+      </c>
+      <c r="B5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" t="s">
+        <v>204</v>
+      </c>
+      <c r="D5">
+        <v>8</v>
+      </c>
+      <c r="E5">
+        <v>7</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>206</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>204</v>
+      </c>
+      <c r="D6">
+        <v>8</v>
+      </c>
+      <c r="E6">
+        <v>7</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>207</v>
+      </c>
+      <c r="B7" t="s">
+        <v>208</v>
+      </c>
+      <c r="C7" t="s">
+        <v>204</v>
+      </c>
+      <c r="D7">
+        <v>8</v>
+      </c>
+      <c r="E7">
+        <v>7</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>209</v>
+      </c>
+      <c r="B8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" t="s">
+        <v>204</v>
+      </c>
+      <c r="D8">
+        <v>16</v>
+      </c>
+      <c r="E8">
+        <v>15</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>210</v>
+      </c>
+      <c r="B9" t="s">
+        <v>211</v>
+      </c>
+      <c r="C9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9">
+        <v>8</v>
+      </c>
+      <c r="E9">
+        <v>7</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>212</v>
+      </c>
+      <c r="B10" t="s">
+        <v>213</v>
+      </c>
+      <c r="C10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10">
+        <v>8</v>
+      </c>
+      <c r="E10">
+        <v>7</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>214</v>
+      </c>
+      <c r="B11" t="s">
+        <v>215</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>216</v>
+      </c>
+      <c r="B12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>217</v>
+      </c>
+      <c r="B13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>8</v>
+      </c>
+      <c r="E13">
+        <v>7</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>218</v>
+      </c>
+      <c r="B14" t="s">
+        <v>160</v>
+      </c>
+      <c r="C14" t="s">
+        <v>219</v>
+      </c>
+      <c r="D14">
+        <v>8</v>
+      </c>
+      <c r="E14">
+        <v>7</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>220</v>
+      </c>
+      <c r="B15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15">
+        <v>8</v>
+      </c>
+      <c r="E15">
+        <v>7</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>221</v>
+      </c>
+      <c r="B16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" t="s">
+        <v>222</v>
+      </c>
+      <c r="D16">
+        <v>8</v>
+      </c>
+      <c r="E16">
+        <v>7</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>223</v>
+      </c>
+      <c r="B17" t="s">
+        <v>172</v>
+      </c>
+      <c r="C17" t="s">
+        <v>224</v>
+      </c>
+      <c r="D17">
+        <v>8</v>
+      </c>
+      <c r="E17">
+        <v>7</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>225</v>
+      </c>
+      <c r="B18" t="s">
+        <v>161</v>
+      </c>
+      <c r="C18" t="s">
+        <v>226</v>
+      </c>
+      <c r="D18">
+        <v>8</v>
+      </c>
+      <c r="E18">
+        <v>7</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>227</v>
+      </c>
+      <c r="B19" t="s">
+        <v>162</v>
+      </c>
+      <c r="C19" t="s">
+        <v>228</v>
+      </c>
+      <c r="D19">
+        <v>8</v>
+      </c>
+      <c r="E19">
+        <v>7</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>229</v>
+      </c>
+      <c r="B20" t="s">
+        <v>230</v>
+      </c>
+      <c r="C20" t="s">
+        <v>231</v>
+      </c>
+      <c r="D20">
+        <v>8</v>
+      </c>
+      <c r="E20">
+        <v>7</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>232</v>
+      </c>
+      <c r="B21" t="s">
+        <v>233</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>8</v>
+      </c>
+      <c r="E21">
+        <v>7</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>234</v>
+      </c>
+      <c r="B22" t="s">
+        <v>118</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>8</v>
+      </c>
+      <c r="E22">
+        <v>7</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>235</v>
+      </c>
+      <c r="B23" t="s">
+        <v>236</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>8</v>
+      </c>
+      <c r="E23">
+        <v>7</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>237</v>
+      </c>
+      <c r="B24" t="s">
+        <v>238</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>8</v>
+      </c>
+      <c r="E24">
+        <v>7</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>239</v>
+      </c>
+      <c r="B25" t="s">
+        <v>240</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>8</v>
+      </c>
+      <c r="E25">
+        <v>7</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>241</v>
+      </c>
+      <c r="B26" t="s">
+        <v>242</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>8</v>
+      </c>
+      <c r="E26">
+        <v>7</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>243</v>
+      </c>
+      <c r="B27" t="s">
+        <v>244</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>8</v>
+      </c>
+      <c r="E27">
+        <v>7</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>245</v>
+      </c>
+      <c r="B28" t="s">
+        <v>246</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>8</v>
+      </c>
+      <c r="E28">
+        <v>7</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>247</v>
+      </c>
+      <c r="B29" t="s">
+        <v>248</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>8</v>
+      </c>
+      <c r="E29">
+        <v>7</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>249</v>
+      </c>
+      <c r="B30" t="s">
+        <v>250</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>8</v>
+      </c>
+      <c r="E30">
+        <v>7</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>251</v>
+      </c>
+      <c r="B31" t="s">
+        <v>252</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>8</v>
+      </c>
+      <c r="E31">
+        <v>7</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>253</v>
+      </c>
+      <c r="B32" t="s">
+        <v>222</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>8</v>
+      </c>
+      <c r="E32">
+        <v>7</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>254</v>
+      </c>
+      <c r="B33" t="s">
+        <v>255</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>8</v>
+      </c>
+      <c r="E33">
+        <v>7</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>256</v>
+      </c>
+      <c r="B34" t="s">
+        <v>257</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <v>8</v>
+      </c>
+      <c r="E34">
+        <v>7</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>258</v>
+      </c>
+      <c r="B35" t="s">
+        <v>259</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>8</v>
+      </c>
+      <c r="E35">
+        <v>7</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>260</v>
+      </c>
+      <c r="B36" t="s">
+        <v>261</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <v>8</v>
+      </c>
+      <c r="E36">
+        <v>7</v>
+      </c>
+      <c r="F36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>262</v>
+      </c>
+      <c r="B37" t="s">
+        <v>263</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <v>8</v>
+      </c>
+      <c r="E37">
+        <v>7</v>
+      </c>
+      <c r="F37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>264</v>
+      </c>
+      <c r="B38" t="s">
+        <v>265</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
+      </c>
+      <c r="D38">
+        <v>8</v>
+      </c>
+      <c r="E38">
+        <v>7</v>
+      </c>
+      <c r="F38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>266</v>
+      </c>
+      <c r="B39" t="s">
+        <v>267</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+      <c r="D39">
+        <v>8</v>
+      </c>
+      <c r="E39">
+        <v>7</v>
+      </c>
+      <c r="F39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>268</v>
+      </c>
+      <c r="B40" t="s">
+        <v>269</v>
+      </c>
+      <c r="C40">
+        <v>0</v>
+      </c>
+      <c r="D40">
+        <v>8</v>
+      </c>
+      <c r="E40">
+        <v>7</v>
+      </c>
+      <c r="F40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>270</v>
+      </c>
+      <c r="B41" t="s">
+        <v>271</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
+      </c>
+      <c r="D41">
+        <v>8</v>
+      </c>
+      <c r="E41">
+        <v>7</v>
+      </c>
+      <c r="F41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>272</v>
+      </c>
+      <c r="B42" t="s">
+        <v>273</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
+      <c r="D42">
+        <v>8</v>
+      </c>
+      <c r="E42">
+        <v>7</v>
+      </c>
+      <c r="F42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>274</v>
+      </c>
+      <c r="B43" t="s">
+        <v>275</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="D43">
+        <v>8</v>
+      </c>
+      <c r="E43">
+        <v>7</v>
+      </c>
+      <c r="F43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>276</v>
+      </c>
+      <c r="B44" t="s">
+        <v>277</v>
+      </c>
+      <c r="C44">
+        <v>0</v>
+      </c>
+      <c r="D44">
+        <v>8</v>
+      </c>
+      <c r="E44">
+        <v>7</v>
+      </c>
+      <c r="F44">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2064,17 +3155,17 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="2" max="2" width="12.54296875" customWidth="1"/>
-    <col min="3" max="3" width="16.453125" customWidth="1"/>
-    <col min="4" max="4" width="9.453125" customWidth="1"/>
-    <col min="5" max="5" width="18.54296875" customWidth="1"/>
-    <col min="6" max="6" width="15.81640625" customWidth="1"/>
+    <col min="2" max="2" width="12.5" customWidth="1"/>
+    <col min="3" max="3" width="16.5" customWidth="1"/>
+    <col min="4" max="4" width="9.5" customWidth="1"/>
+    <col min="5" max="5" width="18.5" customWidth="1"/>
+    <col min="6" max="6" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2094,7 +3185,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>173</v>
       </c>
@@ -2114,7 +3205,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>174</v>
       </c>
@@ -2134,7 +3225,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>175</v>
       </c>
@@ -2154,7 +3245,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>176</v>
       </c>
@@ -2174,7 +3265,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>177</v>
       </c>
@@ -2194,7 +3285,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>200</v>
       </c>
@@ -2214,7 +3305,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>178</v>
       </c>
@@ -2234,7 +3325,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>179</v>
       </c>
@@ -2254,7 +3345,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>180</v>
       </c>
@@ -2274,7 +3365,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>181</v>
       </c>
@@ -2294,7 +3385,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>182</v>
       </c>
@@ -2314,7 +3405,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>184</v>
       </c>
@@ -2348,16 +3439,16 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.453125" customWidth="1"/>
-    <col min="2" max="2" width="13.1796875" customWidth="1"/>
-    <col min="3" max="3" width="13.54296875" customWidth="1"/>
+    <col min="1" max="1" width="22.5" customWidth="1"/>
+    <col min="2" max="2" width="13.1640625" customWidth="1"/>
+    <col min="3" max="3" width="13.5" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="13.1796875" customWidth="1"/>
+    <col min="6" max="6" width="13.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2377,7 +3468,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -2397,7 +3488,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -2417,7 +3508,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -2437,7 +3528,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -2457,7 +3548,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -2477,10 +3568,10 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F12" s="1"/>
     </row>
   </sheetData>
@@ -2496,17 +3587,17 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.453125" customWidth="1"/>
+    <col min="1" max="1" width="19.5" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="16.1796875" customWidth="1"/>
-    <col min="4" max="4" width="10.453125" customWidth="1"/>
-    <col min="5" max="5" width="15.453125" customWidth="1"/>
-    <col min="6" max="6" width="14.453125" customWidth="1"/>
+    <col min="3" max="3" width="16.1640625" customWidth="1"/>
+    <col min="4" max="4" width="10.5" customWidth="1"/>
+    <col min="5" max="5" width="15.5" customWidth="1"/>
+    <col min="6" max="6" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2526,7 +3617,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>72</v>
       </c>
@@ -2546,7 +3637,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>196</v>
       </c>
@@ -2566,7 +3657,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>197</v>
       </c>
@@ -2586,7 +3677,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>198</v>
       </c>
@@ -2619,17 +3710,17 @@
       <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.81640625" customWidth="1"/>
-    <col min="2" max="2" width="14.453125" customWidth="1"/>
-    <col min="3" max="3" width="16.453125" customWidth="1"/>
-    <col min="4" max="4" width="9.81640625" customWidth="1"/>
-    <col min="5" max="5" width="15.453125" customWidth="1"/>
-    <col min="6" max="6" width="14.453125" customWidth="1"/>
+    <col min="1" max="1" width="13.83203125" customWidth="1"/>
+    <col min="2" max="2" width="14.5" customWidth="1"/>
+    <col min="3" max="3" width="16.5" customWidth="1"/>
+    <col min="4" max="4" width="9.83203125" customWidth="1"/>
+    <col min="5" max="5" width="15.5" customWidth="1"/>
+    <col min="6" max="6" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2649,7 +3740,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>92</v>
       </c>
@@ -2669,7 +3760,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>93</v>
       </c>
@@ -2689,7 +3780,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>94</v>
       </c>
@@ -2709,7 +3800,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>95</v>
       </c>
@@ -2729,7 +3820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>96</v>
       </c>
@@ -2749,7 +3840,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>97</v>
       </c>
@@ -2769,7 +3860,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>98</v>
       </c>
@@ -2789,7 +3880,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>99</v>
       </c>
@@ -2809,7 +3900,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>100</v>
       </c>
@@ -2829,7 +3920,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>101</v>
       </c>
@@ -2849,7 +3940,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>102</v>
       </c>
@@ -2869,7 +3960,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>103</v>
       </c>
@@ -2889,7 +3980,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>104</v>
       </c>
@@ -2909,7 +4000,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>105</v>
       </c>
@@ -2929,7 +4020,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>106</v>
       </c>
@@ -2963,16 +4054,16 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.54296875" customWidth="1"/>
-    <col min="2" max="2" width="14.453125" customWidth="1"/>
-    <col min="3" max="3" width="16.81640625" customWidth="1"/>
+    <col min="1" max="1" width="21.5" customWidth="1"/>
+    <col min="2" max="2" width="14.5" customWidth="1"/>
+    <col min="3" max="3" width="16.83203125" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
-    <col min="6" max="6" width="15.453125" customWidth="1"/>
+    <col min="6" max="6" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2992,7 +4083,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>115</v>
       </c>
@@ -3012,7 +4103,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>116</v>
       </c>
@@ -3032,7 +4123,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>117</v>
       </c>
@@ -3065,16 +4156,16 @@
       <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.453125" customWidth="1"/>
-    <col min="2" max="2" width="21.1796875" customWidth="1"/>
-    <col min="3" max="3" width="15.453125" customWidth="1"/>
-    <col min="5" max="5" width="15.1796875" customWidth="1"/>
-    <col min="6" max="6" width="14.1796875" customWidth="1"/>
+    <col min="1" max="1" width="30.5" customWidth="1"/>
+    <col min="2" max="2" width="21.1640625" customWidth="1"/>
+    <col min="3" max="3" width="15.5" customWidth="1"/>
+    <col min="5" max="5" width="15.1640625" customWidth="1"/>
+    <col min="6" max="6" width="14.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3094,7 +4185,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>123</v>
       </c>
@@ -3114,7 +4205,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>124</v>
       </c>
@@ -3134,7 +4225,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>125</v>
       </c>
@@ -3154,7 +4245,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>126</v>
       </c>
@@ -3174,7 +4265,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>127</v>
       </c>
@@ -3194,7 +4285,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>128</v>
       </c>
@@ -3214,7 +4305,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>129</v>
       </c>
@@ -3234,7 +4325,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>130</v>
       </c>
@@ -3254,7 +4345,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>131</v>
       </c>
@@ -3274,7 +4365,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>132</v>
       </c>
@@ -3294,7 +4385,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>133</v>
       </c>
@@ -3314,7 +4405,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>169</v>
       </c>
@@ -3334,7 +4425,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>134</v>
       </c>
@@ -3354,7 +4445,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>135</v>
       </c>
@@ -3374,7 +4465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>136</v>
       </c>
@@ -3394,7 +4485,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>137</v>
       </c>
@@ -3414,7 +4505,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>138</v>
       </c>
@@ -3434,7 +4525,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>139</v>
       </c>
@@ -3454,7 +4545,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>140</v>
       </c>
@@ -3474,7 +4565,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>141</v>
       </c>
@@ -3494,7 +4585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>142</v>
       </c>
@@ -3514,7 +4605,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>143</v>
       </c>
@@ -3534,7 +4625,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>144</v>
       </c>
@@ -3554,7 +4645,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>145</v>
       </c>
@@ -3574,7 +4665,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>146</v>
       </c>
@@ -3594,7 +4685,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>147</v>
       </c>
@@ -3614,7 +4705,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>148</v>
       </c>
@@ -3634,7 +4725,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>149</v>
       </c>
@@ -3654,7 +4745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>150</v>
       </c>
@@ -3674,7 +4765,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>151</v>
       </c>
@@ -3694,7 +4785,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>152</v>
       </c>
@@ -3714,7 +4805,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>153</v>
       </c>
@@ -3734,7 +4825,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>154</v>
       </c>
@@ -3754,7 +4845,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>155</v>
       </c>
@@ -3788,16 +4879,16 @@
       <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.54296875" customWidth="1"/>
-    <col min="2" max="2" width="13.453125" customWidth="1"/>
-    <col min="3" max="3" width="14.453125" customWidth="1"/>
-    <col min="5" max="5" width="14.1796875" customWidth="1"/>
-    <col min="6" max="6" width="13.453125" customWidth="1"/>
+    <col min="1" max="1" width="24.5" customWidth="1"/>
+    <col min="2" max="2" width="13.5" customWidth="1"/>
+    <col min="3" max="3" width="14.5" customWidth="1"/>
+    <col min="5" max="5" width="14.1640625" customWidth="1"/>
+    <col min="6" max="6" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3817,7 +4908,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -3837,7 +4928,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -3857,7 +4948,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -3877,7 +4968,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -3897,7 +4988,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -3917,7 +5008,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -3937,7 +5028,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -3957,7 +5048,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -3977,7 +5068,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -3998,7 +5089,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>114</v>
       </c>
@@ -4018,7 +5109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -4038,7 +5129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -4058,7 +5149,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>39</v>
       </c>
@@ -4078,7 +5169,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>188</v>
       </c>
@@ -4098,7 +5189,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>186</v>
       </c>
@@ -4118,7 +5209,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>189</v>
       </c>
@@ -4138,7 +5229,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>190</v>
       </c>
@@ -4158,7 +5249,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>191</v>
       </c>
@@ -4178,7 +5269,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>192</v>
       </c>
@@ -4198,7 +5289,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>193</v>
       </c>
@@ -4218,7 +5309,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>194</v>
       </c>
@@ -4238,7 +5329,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>195</v>
       </c>
@@ -4272,16 +5363,16 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.453125" customWidth="1"/>
-    <col min="2" max="2" width="13.81640625" customWidth="1"/>
-    <col min="3" max="3" width="15.453125" customWidth="1"/>
-    <col min="5" max="5" width="14.1796875" customWidth="1"/>
-    <col min="6" max="6" width="13.453125" customWidth="1"/>
+    <col min="1" max="1" width="11.5" customWidth="1"/>
+    <col min="2" max="2" width="13.83203125" customWidth="1"/>
+    <col min="3" max="3" width="15.5" customWidth="1"/>
+    <col min="5" max="5" width="14.1640625" customWidth="1"/>
+    <col min="6" max="6" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4301,7 +5392,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -4321,7 +5412,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>39</v>
       </c>
@@ -4341,7 +5432,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>90</v>
       </c>
@@ -4374,16 +5465,16 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.453125" customWidth="1"/>
-    <col min="2" max="2" width="13.453125" customWidth="1"/>
-    <col min="3" max="3" width="15.81640625" customWidth="1"/>
-    <col min="5" max="5" width="14.1796875" customWidth="1"/>
+    <col min="1" max="1" width="11.5" customWidth="1"/>
+    <col min="2" max="2" width="13.5" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" customWidth="1"/>
+    <col min="5" max="5" width="14.1640625" customWidth="1"/>
     <col min="6" max="6" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4403,7 +5494,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -4423,7 +5514,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>39</v>
       </c>
@@ -4443,7 +5534,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>90</v>
       </c>

</xml_diff>

<commit_message>
Fix ADS8686 default values, all must be hex values of the form 0xVALUE
</commit_message>
<xml_diff>
--- a/Registers.xlsx
+++ b/Registers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/koer2434/Google Drive/UST/research/covg/fpga_and_measurements/daq_v2/covg_fpga/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7b0877819b81e9be/Documents/Research Internship/Programs/covg_fpga/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D93E9DF7-F579-BB40-A42C-03166C011540}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{D93E9DF7-F579-BB40-A42C-03166C011540}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D97EF8E7-B776-4AC2-B7B3-9563FF19E8BE}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="22680" windowHeight="19860" firstSheet="5" activeTab="12" xr2:uid="{C3AB243F-651F-4CB0-B6E1-3CA4785EC4D9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="5" activeTab="12" xr2:uid="{C3AB243F-651F-4CB0-B6E1-3CA4785EC4D9}"/>
   </bookViews>
   <sheets>
     <sheet name="I2C" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="706" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="735" uniqueCount="278">
   <si>
     <t>Name</t>
   </si>
@@ -1279,16 +1279,16 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.5" customWidth="1"/>
-    <col min="2" max="2" width="13.1640625" customWidth="1"/>
-    <col min="3" max="3" width="13.5" customWidth="1"/>
+    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="13.1640625" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1308,7 +1308,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1328,7 +1328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -1348,7 +1348,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -1368,7 +1368,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -1388,7 +1388,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -1408,10 +1408,10 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F12" s="1"/>
     </row>
   </sheetData>
@@ -1427,16 +1427,16 @@
       <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.5" customWidth="1"/>
-    <col min="2" max="2" width="15.1640625" customWidth="1"/>
-    <col min="3" max="3" width="16.5" customWidth="1"/>
-    <col min="5" max="5" width="14.5" customWidth="1"/>
-    <col min="6" max="6" width="14.1640625" customWidth="1"/>
+    <col min="1" max="1" width="26.42578125" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1456,7 +1456,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>43</v>
       </c>
@@ -1476,7 +1476,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>87</v>
       </c>
@@ -1496,7 +1496,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>44</v>
       </c>
@@ -1516,7 +1516,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>72</v>
       </c>
@@ -1536,7 +1536,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>45</v>
       </c>
@@ -1556,7 +1556,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -1576,7 +1576,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>46</v>
       </c>
@@ -1596,7 +1596,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>47</v>
       </c>
@@ -1616,7 +1616,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>48</v>
       </c>
@@ -1636,7 +1636,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>49</v>
       </c>
@@ -1656,7 +1656,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>50</v>
       </c>
@@ -1676,7 +1676,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>51</v>
       </c>
@@ -1696,7 +1696,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>52</v>
       </c>
@@ -1716,7 +1716,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>53</v>
       </c>
@@ -1736,7 +1736,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>54</v>
       </c>
@@ -1756,7 +1756,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>55</v>
       </c>
@@ -1776,7 +1776,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>73</v>
       </c>
@@ -1796,7 +1796,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>74</v>
       </c>
@@ -1816,7 +1816,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>75</v>
       </c>
@@ -1836,7 +1836,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>76</v>
       </c>
@@ -1856,7 +1856,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>77</v>
       </c>
@@ -1876,7 +1876,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>78</v>
       </c>
@@ -1896,7 +1896,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>79</v>
       </c>
@@ -1916,7 +1916,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>80</v>
       </c>
@@ -1936,7 +1936,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>81</v>
       </c>
@@ -1956,7 +1956,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>82</v>
       </c>
@@ -1976,7 +1976,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>83</v>
       </c>
@@ -1996,7 +1996,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>84</v>
       </c>
@@ -2016,7 +2016,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>85</v>
       </c>
@@ -2036,7 +2036,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>86</v>
       </c>
@@ -2056,7 +2056,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>109</v>
       </c>
@@ -2076,7 +2076,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>108</v>
       </c>
@@ -2096,7 +2096,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>110</v>
       </c>
@@ -2116,7 +2116,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>111</v>
       </c>
@@ -2136,7 +2136,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>113</v>
       </c>
@@ -2156,7 +2156,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>112</v>
       </c>
@@ -2190,9 +2190,9 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2225,9 +2225,9 @@
       <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2256,13 +2256,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1CC0846-B885-4A4F-9321-B09606FEAD42}">
   <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F44"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C22" sqref="C21:C44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="18.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2282,15 +2285,15 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>201</v>
       </c>
       <c r="B2" t="s">
         <v>18</v>
       </c>
-      <c r="C2">
-        <v>0</v>
+      <c r="C2" t="s">
+        <v>6</v>
       </c>
       <c r="D2">
         <v>8</v>
@@ -2302,15 +2305,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>202</v>
       </c>
       <c r="B3" t="s">
         <v>107</v>
       </c>
-      <c r="C3">
-        <v>0</v>
+      <c r="C3" t="s">
+        <v>6</v>
       </c>
       <c r="D3">
         <v>8</v>
@@ -2322,7 +2325,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>203</v>
       </c>
@@ -2342,7 +2345,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>205</v>
       </c>
@@ -2362,7 +2365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>206</v>
       </c>
@@ -2382,7 +2385,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>207</v>
       </c>
@@ -2402,7 +2405,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>209</v>
       </c>
@@ -2422,7 +2425,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>210</v>
       </c>
@@ -2442,7 +2445,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>212</v>
       </c>
@@ -2462,15 +2465,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>214</v>
       </c>
       <c r="B11" t="s">
         <v>215</v>
       </c>
-      <c r="C11">
-        <v>0</v>
+      <c r="C11" t="s">
+        <v>6</v>
       </c>
       <c r="D11">
         <v>2</v>
@@ -2482,15 +2485,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>216</v>
       </c>
       <c r="B12" t="s">
         <v>33</v>
       </c>
-      <c r="C12">
-        <v>2</v>
+      <c r="C12" t="s">
+        <v>18</v>
       </c>
       <c r="D12">
         <v>2</v>
@@ -2502,15 +2505,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>217</v>
       </c>
       <c r="B13" t="s">
         <v>8</v>
       </c>
-      <c r="C13">
-        <v>0</v>
+      <c r="C13" t="s">
+        <v>6</v>
       </c>
       <c r="D13">
         <v>8</v>
@@ -2522,7 +2525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>218</v>
       </c>
@@ -2542,7 +2545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>220</v>
       </c>
@@ -2562,7 +2565,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>221</v>
       </c>
@@ -2582,7 +2585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>223</v>
       </c>
@@ -2602,7 +2605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>225</v>
       </c>
@@ -2622,7 +2625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>227</v>
       </c>
@@ -2642,7 +2645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>229</v>
       </c>
@@ -2662,15 +2665,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>232</v>
       </c>
       <c r="B21" t="s">
         <v>233</v>
       </c>
-      <c r="C21">
-        <v>0</v>
+      <c r="C21" t="s">
+        <v>6</v>
       </c>
       <c r="D21">
         <v>8</v>
@@ -2682,15 +2685,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>234</v>
       </c>
       <c r="B22" t="s">
         <v>118</v>
       </c>
-      <c r="C22">
-        <v>0</v>
+      <c r="C22" t="s">
+        <v>6</v>
       </c>
       <c r="D22">
         <v>8</v>
@@ -2702,15 +2705,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>235</v>
       </c>
       <c r="B23" t="s">
         <v>236</v>
       </c>
-      <c r="C23">
-        <v>0</v>
+      <c r="C23" t="s">
+        <v>6</v>
       </c>
       <c r="D23">
         <v>8</v>
@@ -2722,15 +2725,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>237</v>
       </c>
       <c r="B24" t="s">
         <v>238</v>
       </c>
-      <c r="C24">
-        <v>0</v>
+      <c r="C24" t="s">
+        <v>6</v>
       </c>
       <c r="D24">
         <v>8</v>
@@ -2742,15 +2745,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>239</v>
       </c>
       <c r="B25" t="s">
         <v>240</v>
       </c>
-      <c r="C25">
-        <v>0</v>
+      <c r="C25" t="s">
+        <v>6</v>
       </c>
       <c r="D25">
         <v>8</v>
@@ -2762,15 +2765,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>241</v>
       </c>
       <c r="B26" t="s">
         <v>242</v>
       </c>
-      <c r="C26">
-        <v>0</v>
+      <c r="C26" t="s">
+        <v>6</v>
       </c>
       <c r="D26">
         <v>8</v>
@@ -2782,15 +2785,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>243</v>
       </c>
       <c r="B27" t="s">
         <v>244</v>
       </c>
-      <c r="C27">
-        <v>0</v>
+      <c r="C27" t="s">
+        <v>6</v>
       </c>
       <c r="D27">
         <v>8</v>
@@ -2802,15 +2805,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>245</v>
       </c>
       <c r="B28" t="s">
         <v>246</v>
       </c>
-      <c r="C28">
-        <v>0</v>
+      <c r="C28" t="s">
+        <v>6</v>
       </c>
       <c r="D28">
         <v>8</v>
@@ -2822,15 +2825,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>247</v>
       </c>
       <c r="B29" t="s">
         <v>248</v>
       </c>
-      <c r="C29">
-        <v>0</v>
+      <c r="C29" t="s">
+        <v>6</v>
       </c>
       <c r="D29">
         <v>8</v>
@@ -2842,15 +2845,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>249</v>
       </c>
       <c r="B30" t="s">
         <v>250</v>
       </c>
-      <c r="C30">
-        <v>0</v>
+      <c r="C30" t="s">
+        <v>6</v>
       </c>
       <c r="D30">
         <v>8</v>
@@ -2862,15 +2865,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>251</v>
       </c>
       <c r="B31" t="s">
         <v>252</v>
       </c>
-      <c r="C31">
-        <v>0</v>
+      <c r="C31" t="s">
+        <v>6</v>
       </c>
       <c r="D31">
         <v>8</v>
@@ -2882,15 +2885,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>253</v>
       </c>
       <c r="B32" t="s">
         <v>222</v>
       </c>
-      <c r="C32">
-        <v>0</v>
+      <c r="C32" t="s">
+        <v>6</v>
       </c>
       <c r="D32">
         <v>8</v>
@@ -2902,15 +2905,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>254</v>
       </c>
       <c r="B33" t="s">
         <v>255</v>
       </c>
-      <c r="C33">
-        <v>0</v>
+      <c r="C33" t="s">
+        <v>6</v>
       </c>
       <c r="D33">
         <v>8</v>
@@ -2922,15 +2925,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>256</v>
       </c>
       <c r="B34" t="s">
         <v>257</v>
       </c>
-      <c r="C34">
-        <v>0</v>
+      <c r="C34" t="s">
+        <v>6</v>
       </c>
       <c r="D34">
         <v>8</v>
@@ -2942,15 +2945,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>258</v>
       </c>
       <c r="B35" t="s">
         <v>259</v>
       </c>
-      <c r="C35">
-        <v>0</v>
+      <c r="C35" t="s">
+        <v>6</v>
       </c>
       <c r="D35">
         <v>8</v>
@@ -2962,15 +2965,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>260</v>
       </c>
       <c r="B36" t="s">
         <v>261</v>
       </c>
-      <c r="C36">
-        <v>0</v>
+      <c r="C36" t="s">
+        <v>6</v>
       </c>
       <c r="D36">
         <v>8</v>
@@ -2982,15 +2985,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>262</v>
       </c>
       <c r="B37" t="s">
         <v>263</v>
       </c>
-      <c r="C37">
-        <v>0</v>
+      <c r="C37" t="s">
+        <v>6</v>
       </c>
       <c r="D37">
         <v>8</v>
@@ -3002,15 +3005,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>264</v>
       </c>
       <c r="B38" t="s">
         <v>265</v>
       </c>
-      <c r="C38">
-        <v>0</v>
+      <c r="C38" t="s">
+        <v>6</v>
       </c>
       <c r="D38">
         <v>8</v>
@@ -3022,15 +3025,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>266</v>
       </c>
       <c r="B39" t="s">
         <v>267</v>
       </c>
-      <c r="C39">
-        <v>0</v>
+      <c r="C39" t="s">
+        <v>6</v>
       </c>
       <c r="D39">
         <v>8</v>
@@ -3042,15 +3045,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>268</v>
       </c>
       <c r="B40" t="s">
         <v>269</v>
       </c>
-      <c r="C40">
-        <v>0</v>
+      <c r="C40" t="s">
+        <v>6</v>
       </c>
       <c r="D40">
         <v>8</v>
@@ -3062,15 +3065,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>270</v>
       </c>
       <c r="B41" t="s">
         <v>271</v>
       </c>
-      <c r="C41">
-        <v>0</v>
+      <c r="C41" t="s">
+        <v>6</v>
       </c>
       <c r="D41">
         <v>8</v>
@@ -3082,15 +3085,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>272</v>
       </c>
       <c r="B42" t="s">
         <v>273</v>
       </c>
-      <c r="C42">
-        <v>0</v>
+      <c r="C42" t="s">
+        <v>6</v>
       </c>
       <c r="D42">
         <v>8</v>
@@ -3102,15 +3105,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>274</v>
       </c>
       <c r="B43" t="s">
         <v>275</v>
       </c>
-      <c r="C43">
-        <v>0</v>
+      <c r="C43" t="s">
+        <v>6</v>
       </c>
       <c r="D43">
         <v>8</v>
@@ -3122,15 +3125,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>276</v>
       </c>
       <c r="B44" t="s">
         <v>277</v>
       </c>
-      <c r="C44">
-        <v>0</v>
+      <c r="C44" t="s">
+        <v>6</v>
       </c>
       <c r="D44">
         <v>8</v>
@@ -3143,6 +3146,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3155,17 +3159,17 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="2" max="2" width="12.5" customWidth="1"/>
-    <col min="3" max="3" width="16.5" customWidth="1"/>
-    <col min="4" max="4" width="9.5" customWidth="1"/>
-    <col min="5" max="5" width="18.5" customWidth="1"/>
-    <col min="6" max="6" width="15.83203125" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3185,7 +3189,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>173</v>
       </c>
@@ -3205,7 +3209,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>174</v>
       </c>
@@ -3225,7 +3229,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>175</v>
       </c>
@@ -3245,7 +3249,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>176</v>
       </c>
@@ -3265,7 +3269,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>177</v>
       </c>
@@ -3285,7 +3289,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>200</v>
       </c>
@@ -3305,7 +3309,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>178</v>
       </c>
@@ -3325,7 +3329,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>179</v>
       </c>
@@ -3345,7 +3349,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>180</v>
       </c>
@@ -3365,7 +3369,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>181</v>
       </c>
@@ -3385,7 +3389,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>182</v>
       </c>
@@ -3405,7 +3409,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>184</v>
       </c>
@@ -3439,16 +3443,16 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.5" customWidth="1"/>
-    <col min="2" max="2" width="13.1640625" customWidth="1"/>
-    <col min="3" max="3" width="13.5" customWidth="1"/>
+    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="13.1640625" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3468,7 +3472,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -3488,7 +3492,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -3508,7 +3512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -3528,7 +3532,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -3548,7 +3552,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -3568,10 +3572,10 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F12" s="1"/>
     </row>
   </sheetData>
@@ -3587,17 +3591,17 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.5" customWidth="1"/>
+    <col min="1" max="1" width="19.42578125" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="16.1640625" customWidth="1"/>
-    <col min="4" max="4" width="10.5" customWidth="1"/>
-    <col min="5" max="5" width="15.5" customWidth="1"/>
-    <col min="6" max="6" width="14.5" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3617,7 +3621,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>72</v>
       </c>
@@ -3637,7 +3641,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>196</v>
       </c>
@@ -3657,7 +3661,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>197</v>
       </c>
@@ -3677,7 +3681,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>198</v>
       </c>
@@ -3710,17 +3714,17 @@
       <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.83203125" customWidth="1"/>
-    <col min="2" max="2" width="14.5" customWidth="1"/>
-    <col min="3" max="3" width="16.5" customWidth="1"/>
-    <col min="4" max="4" width="9.83203125" customWidth="1"/>
-    <col min="5" max="5" width="15.5" customWidth="1"/>
-    <col min="6" max="6" width="14.5" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3740,7 +3744,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>92</v>
       </c>
@@ -3760,7 +3764,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>93</v>
       </c>
@@ -3780,7 +3784,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>94</v>
       </c>
@@ -3800,7 +3804,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>95</v>
       </c>
@@ -3820,7 +3824,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>96</v>
       </c>
@@ -3840,7 +3844,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>97</v>
       </c>
@@ -3860,7 +3864,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>98</v>
       </c>
@@ -3880,7 +3884,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>99</v>
       </c>
@@ -3900,7 +3904,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>100</v>
       </c>
@@ -3920,7 +3924,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>101</v>
       </c>
@@ -3940,7 +3944,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>102</v>
       </c>
@@ -3960,7 +3964,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>103</v>
       </c>
@@ -3980,7 +3984,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>104</v>
       </c>
@@ -4000,7 +4004,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>105</v>
       </c>
@@ -4020,7 +4024,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>106</v>
       </c>
@@ -4054,16 +4058,16 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.5" customWidth="1"/>
-    <col min="2" max="2" width="14.5" customWidth="1"/>
-    <col min="3" max="3" width="16.83203125" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
-    <col min="6" max="6" width="15.5" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4083,7 +4087,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>115</v>
       </c>
@@ -4103,7 +4107,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>116</v>
       </c>
@@ -4123,7 +4127,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>117</v>
       </c>
@@ -4156,16 +4160,16 @@
       <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.5" customWidth="1"/>
-    <col min="2" max="2" width="21.1640625" customWidth="1"/>
-    <col min="3" max="3" width="15.5" customWidth="1"/>
-    <col min="5" max="5" width="15.1640625" customWidth="1"/>
-    <col min="6" max="6" width="14.1640625" customWidth="1"/>
+    <col min="1" max="1" width="30.42578125" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4185,7 +4189,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>123</v>
       </c>
@@ -4205,7 +4209,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>124</v>
       </c>
@@ -4225,7 +4229,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>125</v>
       </c>
@@ -4245,7 +4249,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>126</v>
       </c>
@@ -4265,7 +4269,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>127</v>
       </c>
@@ -4285,7 +4289,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>128</v>
       </c>
@@ -4305,7 +4309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>129</v>
       </c>
@@ -4325,7 +4329,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>130</v>
       </c>
@@ -4345,7 +4349,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>131</v>
       </c>
@@ -4365,7 +4369,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>132</v>
       </c>
@@ -4385,7 +4389,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>133</v>
       </c>
@@ -4405,7 +4409,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>169</v>
       </c>
@@ -4425,7 +4429,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>134</v>
       </c>
@@ -4445,7 +4449,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>135</v>
       </c>
@@ -4465,7 +4469,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>136</v>
       </c>
@@ -4485,7 +4489,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>137</v>
       </c>
@@ -4505,7 +4509,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>138</v>
       </c>
@@ -4525,7 +4529,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>139</v>
       </c>
@@ -4545,7 +4549,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>140</v>
       </c>
@@ -4565,7 +4569,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>141</v>
       </c>
@@ -4585,7 +4589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>142</v>
       </c>
@@ -4605,7 +4609,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>143</v>
       </c>
@@ -4625,7 +4629,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>144</v>
       </c>
@@ -4645,7 +4649,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>145</v>
       </c>
@@ -4665,7 +4669,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>146</v>
       </c>
@@ -4685,7 +4689,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>147</v>
       </c>
@@ -4705,7 +4709,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>148</v>
       </c>
@@ -4725,7 +4729,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>149</v>
       </c>
@@ -4745,7 +4749,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>150</v>
       </c>
@@ -4765,7 +4769,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>151</v>
       </c>
@@ -4785,7 +4789,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>152</v>
       </c>
@@ -4805,7 +4809,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>153</v>
       </c>
@@ -4825,7 +4829,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>154</v>
       </c>
@@ -4845,7 +4849,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>155</v>
       </c>
@@ -4879,16 +4883,16 @@
       <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.5" customWidth="1"/>
-    <col min="2" max="2" width="13.5" customWidth="1"/>
-    <col min="3" max="3" width="14.5" customWidth="1"/>
-    <col min="5" max="5" width="14.1640625" customWidth="1"/>
-    <col min="6" max="6" width="13.5" customWidth="1"/>
+    <col min="1" max="1" width="24.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4908,7 +4912,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -4928,7 +4932,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -4948,7 +4952,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -4968,7 +4972,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -4988,7 +4992,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -5008,7 +5012,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -5028,7 +5032,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -5048,7 +5052,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -5068,7 +5072,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -5089,7 +5093,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>114</v>
       </c>
@@ -5109,7 +5113,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -5129,7 +5133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -5149,7 +5153,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>39</v>
       </c>
@@ -5169,7 +5173,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>188</v>
       </c>
@@ -5189,7 +5193,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>186</v>
       </c>
@@ -5209,7 +5213,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>189</v>
       </c>
@@ -5229,7 +5233,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>190</v>
       </c>
@@ -5249,7 +5253,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>191</v>
       </c>
@@ -5269,7 +5273,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>192</v>
       </c>
@@ -5289,7 +5293,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>193</v>
       </c>
@@ -5309,7 +5313,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>194</v>
       </c>
@@ -5329,7 +5333,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>195</v>
       </c>
@@ -5363,16 +5367,16 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5" customWidth="1"/>
-    <col min="2" max="2" width="13.83203125" customWidth="1"/>
-    <col min="3" max="3" width="15.5" customWidth="1"/>
-    <col min="5" max="5" width="14.1640625" customWidth="1"/>
-    <col min="6" max="6" width="13.5" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5392,7 +5396,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -5412,7 +5416,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>39</v>
       </c>
@@ -5432,7 +5436,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>90</v>
       </c>
@@ -5465,16 +5469,16 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5" customWidth="1"/>
-    <col min="2" max="2" width="13.5" customWidth="1"/>
-    <col min="3" max="3" width="15.83203125" customWidth="1"/>
-    <col min="5" max="5" width="14.1640625" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" customWidth="1"/>
     <col min="6" max="6" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5494,7 +5498,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -5514,7 +5518,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>39</v>
       </c>
@@ -5534,7 +5538,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>90</v>
       </c>

</xml_diff>

<commit_message>
Remove unecessary Registers sheets
</commit_message>
<xml_diff>
--- a/Registers.xlsx
+++ b/Registers.xlsx
@@ -8,29 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7b0877819b81e9be/Documents/Research Internship/Programs/covg_fpga/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{D93E9DF7-F579-BB40-A42C-03166C011540}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D97EF8E7-B776-4AC2-B7B3-9563FF19E8BE}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{D93E9DF7-F579-BB40-A42C-03166C011540}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4C4BB808-75A3-462F-820C-7B025560BB99}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="5" activeTab="12" xr2:uid="{C3AB243F-651F-4CB0-B6E1-3CA4785EC4D9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="10" xr2:uid="{C3AB243F-651F-4CB0-B6E1-3CA4785EC4D9}"/>
   </bookViews>
   <sheets>
     <sheet name="I2C" sheetId="1" r:id="rId1"/>
-    <sheet name="I2C_NEW" sheetId="12" r:id="rId2"/>
-    <sheet name="TCA9555" sheetId="3" r:id="rId3"/>
-    <sheet name="clamp_configuration" sheetId="8" r:id="rId4"/>
-    <sheet name="24AA025UID" sheetId="9" r:id="rId5"/>
-    <sheet name="DAC53401" sheetId="10" r:id="rId6"/>
-    <sheet name="SPI" sheetId="2" r:id="rId7"/>
-    <sheet name="SPI_WB_1" sheetId="4" r:id="rId8"/>
-    <sheet name="SPI_WB_2" sheetId="5" r:id="rId9"/>
-    <sheet name="DAC80508" sheetId="6" r:id="rId10"/>
-    <sheet name="AD5453" sheetId="14" r:id="rId11"/>
-    <sheet name="ADS7952" sheetId="15" r:id="rId12"/>
-    <sheet name="ADS8686" sheetId="16" r:id="rId13"/>
-    <sheet name="AD7961" sheetId="13" r:id="rId14"/>
+    <sheet name="TCA9555" sheetId="3" r:id="rId2"/>
+    <sheet name="clamp_configuration" sheetId="8" r:id="rId3"/>
+    <sheet name="24AA025UID" sheetId="9" r:id="rId4"/>
+    <sheet name="DAC53401" sheetId="10" r:id="rId5"/>
+    <sheet name="SPI" sheetId="2" r:id="rId6"/>
+    <sheet name="DAC80508" sheetId="6" r:id="rId7"/>
+    <sheet name="AD5453" sheetId="14" r:id="rId8"/>
+    <sheet name="ADS7952" sheetId="15" r:id="rId9"/>
+    <sheet name="ADS8686" sheetId="16" r:id="rId10"/>
+    <sheet name="AD7961" sheetId="13" r:id="rId11"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">I2C!$A$1:$E$6</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">I2C_NEW!$A$1:$E$6</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -51,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="735" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="276">
   <si>
     <t>Name</t>
   </si>
@@ -323,9 +319,6 @@
     <t>Bit Index (Low)</t>
   </si>
   <si>
-    <t>TRIGGER_BIT</t>
-  </si>
-  <si>
     <t>0x0816</t>
   </si>
   <si>
@@ -561,9 +554,6 @@
   </si>
   <si>
     <t>DAC_PDN</t>
-  </si>
-  <si>
-    <t>0x50</t>
   </si>
   <si>
     <t>0x70</t>
@@ -1420,843 +1410,10 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C9C2D46-1736-43E0-82AF-3E209A55AC59}">
-  <dimension ref="A1:F37"/>
-  <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="26.42578125" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" customWidth="1"/>
-    <col min="6" max="6" width="14.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>88</v>
-      </c>
-      <c r="F1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D2">
-        <v>16</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>87</v>
-      </c>
-      <c r="B3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C3" t="s">
-        <v>91</v>
-      </c>
-      <c r="D3">
-        <v>16</v>
-      </c>
-      <c r="E3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C4" t="s">
-        <v>71</v>
-      </c>
-      <c r="D4">
-        <v>16</v>
-      </c>
-      <c r="E4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>72</v>
-      </c>
-      <c r="B5" t="s">
-        <v>58</v>
-      </c>
-      <c r="C5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D5">
-        <v>16</v>
-      </c>
-      <c r="E5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>45</v>
-      </c>
-      <c r="B6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D6">
-        <v>16</v>
-      </c>
-      <c r="E6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B7" t="s">
-        <v>60</v>
-      </c>
-      <c r="C7" t="s">
-        <v>38</v>
-      </c>
-      <c r="D7">
-        <v>16</v>
-      </c>
-      <c r="E7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>46</v>
-      </c>
-      <c r="B8" t="s">
-        <v>61</v>
-      </c>
-      <c r="C8" t="s">
-        <v>38</v>
-      </c>
-      <c r="D8">
-        <v>16</v>
-      </c>
-      <c r="E8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>47</v>
-      </c>
-      <c r="B9" t="s">
-        <v>62</v>
-      </c>
-      <c r="C9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D9">
-        <v>16</v>
-      </c>
-      <c r="E9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>48</v>
-      </c>
-      <c r="B10" t="s">
-        <v>63</v>
-      </c>
-      <c r="C10" t="s">
-        <v>38</v>
-      </c>
-      <c r="D10">
-        <v>16</v>
-      </c>
-      <c r="E10" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>49</v>
-      </c>
-      <c r="B11" t="s">
-        <v>64</v>
-      </c>
-      <c r="C11" t="s">
-        <v>38</v>
-      </c>
-      <c r="D11">
-        <v>16</v>
-      </c>
-      <c r="E11" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>50</v>
-      </c>
-      <c r="B12" t="s">
-        <v>65</v>
-      </c>
-      <c r="C12" t="s">
-        <v>38</v>
-      </c>
-      <c r="D12">
-        <v>16</v>
-      </c>
-      <c r="E12" t="s">
-        <v>9</v>
-      </c>
-      <c r="F12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>51</v>
-      </c>
-      <c r="B13" t="s">
-        <v>66</v>
-      </c>
-      <c r="C13" t="s">
-        <v>38</v>
-      </c>
-      <c r="D13">
-        <v>16</v>
-      </c>
-      <c r="E13" t="s">
-        <v>9</v>
-      </c>
-      <c r="F13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>52</v>
-      </c>
-      <c r="B14" t="s">
-        <v>67</v>
-      </c>
-      <c r="C14" t="s">
-        <v>38</v>
-      </c>
-      <c r="D14">
-        <v>16</v>
-      </c>
-      <c r="E14" t="s">
-        <v>9</v>
-      </c>
-      <c r="F14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>53</v>
-      </c>
-      <c r="B15" t="s">
-        <v>68</v>
-      </c>
-      <c r="C15" t="s">
-        <v>38</v>
-      </c>
-      <c r="D15">
-        <v>16</v>
-      </c>
-      <c r="E15" t="s">
-        <v>9</v>
-      </c>
-      <c r="F15" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>54</v>
-      </c>
-      <c r="B16" t="s">
-        <v>69</v>
-      </c>
-      <c r="C16" t="s">
-        <v>38</v>
-      </c>
-      <c r="D16">
-        <v>16</v>
-      </c>
-      <c r="E16" t="s">
-        <v>9</v>
-      </c>
-      <c r="F16" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>55</v>
-      </c>
-      <c r="B17" t="s">
-        <v>70</v>
-      </c>
-      <c r="C17" t="s">
-        <v>38</v>
-      </c>
-      <c r="D17">
-        <v>16</v>
-      </c>
-      <c r="E17" t="s">
-        <v>9</v>
-      </c>
-      <c r="F17" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>73</v>
-      </c>
-      <c r="B18" t="s">
-        <v>58</v>
-      </c>
-      <c r="C18" t="s">
-        <v>37</v>
-      </c>
-      <c r="D18">
-        <v>1</v>
-      </c>
-      <c r="E18">
-        <v>13</v>
-      </c>
-      <c r="F18">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>74</v>
-      </c>
-      <c r="B19" t="s">
-        <v>58</v>
-      </c>
-      <c r="C19" t="s">
-        <v>37</v>
-      </c>
-      <c r="D19">
-        <v>1</v>
-      </c>
-      <c r="E19">
-        <v>12</v>
-      </c>
-      <c r="F19">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>75</v>
-      </c>
-      <c r="B20" t="s">
-        <v>58</v>
-      </c>
-      <c r="C20" t="s">
-        <v>37</v>
-      </c>
-      <c r="D20">
-        <v>1</v>
-      </c>
-      <c r="E20">
-        <v>11</v>
-      </c>
-      <c r="F20">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>76</v>
-      </c>
-      <c r="B21" t="s">
-        <v>58</v>
-      </c>
-      <c r="C21" t="s">
-        <v>37</v>
-      </c>
-      <c r="D21">
-        <v>1</v>
-      </c>
-      <c r="E21">
-        <v>10</v>
-      </c>
-      <c r="F21">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>77</v>
-      </c>
-      <c r="B22" t="s">
-        <v>58</v>
-      </c>
-      <c r="C22" t="s">
-        <v>37</v>
-      </c>
-      <c r="D22">
-        <v>1</v>
-      </c>
-      <c r="E22">
-        <v>9</v>
-      </c>
-      <c r="F22">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>78</v>
-      </c>
-      <c r="B23" t="s">
-        <v>58</v>
-      </c>
-      <c r="C23" t="s">
-        <v>37</v>
-      </c>
-      <c r="D23">
-        <v>1</v>
-      </c>
-      <c r="E23">
-        <v>8</v>
-      </c>
-      <c r="F23">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>79</v>
-      </c>
-      <c r="B24" t="s">
-        <v>58</v>
-      </c>
-      <c r="C24" t="s">
-        <v>37</v>
-      </c>
-      <c r="D24">
-        <v>1</v>
-      </c>
-      <c r="E24">
-        <v>7</v>
-      </c>
-      <c r="F24">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>80</v>
-      </c>
-      <c r="B25" t="s">
-        <v>58</v>
-      </c>
-      <c r="C25" t="s">
-        <v>37</v>
-      </c>
-      <c r="D25">
-        <v>1</v>
-      </c>
-      <c r="E25">
-        <v>6</v>
-      </c>
-      <c r="F25">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>81</v>
-      </c>
-      <c r="B26" t="s">
-        <v>58</v>
-      </c>
-      <c r="C26" t="s">
-        <v>37</v>
-      </c>
-      <c r="D26">
-        <v>1</v>
-      </c>
-      <c r="E26">
-        <v>5</v>
-      </c>
-      <c r="F26">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>82</v>
-      </c>
-      <c r="B27" t="s">
-        <v>58</v>
-      </c>
-      <c r="C27" t="s">
-        <v>37</v>
-      </c>
-      <c r="D27">
-        <v>1</v>
-      </c>
-      <c r="E27">
-        <v>4</v>
-      </c>
-      <c r="F27">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>83</v>
-      </c>
-      <c r="B28" t="s">
-        <v>58</v>
-      </c>
-      <c r="C28" t="s">
-        <v>37</v>
-      </c>
-      <c r="D28">
-        <v>1</v>
-      </c>
-      <c r="E28">
-        <v>3</v>
-      </c>
-      <c r="F28">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>84</v>
-      </c>
-      <c r="B29" t="s">
-        <v>58</v>
-      </c>
-      <c r="C29" t="s">
-        <v>37</v>
-      </c>
-      <c r="D29">
-        <v>1</v>
-      </c>
-      <c r="E29">
-        <v>2</v>
-      </c>
-      <c r="F29">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>85</v>
-      </c>
-      <c r="B30" t="s">
-        <v>58</v>
-      </c>
-      <c r="C30" t="s">
-        <v>37</v>
-      </c>
-      <c r="D30">
-        <v>1</v>
-      </c>
-      <c r="E30">
-        <v>1</v>
-      </c>
-      <c r="F30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>86</v>
-      </c>
-      <c r="B31" t="s">
-        <v>58</v>
-      </c>
-      <c r="C31" t="s">
-        <v>37</v>
-      </c>
-      <c r="D31">
-        <v>1</v>
-      </c>
-      <c r="E31">
-        <v>0</v>
-      </c>
-      <c r="F31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>109</v>
-      </c>
-      <c r="B32" t="s">
-        <v>107</v>
-      </c>
-      <c r="C32" t="s">
-        <v>10</v>
-      </c>
-      <c r="D32">
-        <v>32</v>
-      </c>
-      <c r="E32" t="s">
-        <v>9</v>
-      </c>
-      <c r="F32" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>108</v>
-      </c>
-      <c r="B33" t="s">
-        <v>30</v>
-      </c>
-      <c r="C33" t="s">
-        <v>10</v>
-      </c>
-      <c r="D33">
-        <v>32</v>
-      </c>
-      <c r="E33" t="s">
-        <v>9</v>
-      </c>
-      <c r="F33" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>110</v>
-      </c>
-      <c r="B34" t="s">
-        <v>40</v>
-      </c>
-      <c r="C34" t="s">
-        <v>10</v>
-      </c>
-      <c r="D34">
-        <v>32</v>
-      </c>
-      <c r="E34" t="s">
-        <v>9</v>
-      </c>
-      <c r="F34" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>111</v>
-      </c>
-      <c r="B35" t="s">
-        <v>42</v>
-      </c>
-      <c r="C35" t="s">
-        <v>10</v>
-      </c>
-      <c r="D35">
-        <v>32</v>
-      </c>
-      <c r="E35" t="s">
-        <v>9</v>
-      </c>
-      <c r="F35" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>113</v>
-      </c>
-      <c r="B36" t="s">
-        <v>4</v>
-      </c>
-      <c r="C36" t="s">
-        <v>37</v>
-      </c>
-      <c r="D36">
-        <v>1</v>
-      </c>
-      <c r="E36">
-        <v>8</v>
-      </c>
-      <c r="F36">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>112</v>
-      </c>
-      <c r="B37" t="s">
-        <v>4</v>
-      </c>
-      <c r="C37" t="s">
-        <v>37</v>
-      </c>
-      <c r="D37">
-        <v>1</v>
-      </c>
-      <c r="E37">
-        <v>9</v>
-      </c>
-      <c r="F37">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{427C2A19-8BF7-4B8D-9492-08A4DEB2EF8C}">
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>88</v>
-      </c>
-      <c r="F1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9F9F601-34D5-480B-81CE-67CE1CDB2EB8}">
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>88</v>
-      </c>
-      <c r="F1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1CC0846-B885-4A4F-9321-B09606FEAD42}">
   <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="C22" sqref="C21:C44"/>
     </sheetView>
   </sheetViews>
@@ -2287,7 +1444,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B2" t="s">
         <v>18</v>
@@ -2307,10 +1464,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
@@ -2327,13 +1484,13 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B4" t="s">
         <v>30</v>
       </c>
       <c r="C4" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D4">
         <v>8</v>
@@ -2347,13 +1504,13 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B5" t="s">
         <v>41</v>
       </c>
       <c r="C5" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D5">
         <v>8</v>
@@ -2367,13 +1524,13 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B6" t="s">
         <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D6">
         <v>8</v>
@@ -2387,13 +1544,13 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B7" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C7" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D7">
         <v>8</v>
@@ -2407,13 +1564,13 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B8" t="s">
         <v>31</v>
       </c>
       <c r="C8" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D8">
         <v>16</v>
@@ -2427,10 +1584,10 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B9" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C9" t="s">
         <v>6</v>
@@ -2447,10 +1604,10 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B10" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C10" t="s">
         <v>6</v>
@@ -2467,10 +1624,10 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B11" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C11" t="s">
         <v>6</v>
@@ -2487,7 +1644,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B12" t="s">
         <v>33</v>
@@ -2507,7 +1664,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B13" t="s">
         <v>8</v>
@@ -2527,13 +1684,13 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C14" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D14">
         <v>8</v>
@@ -2547,7 +1704,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B15" t="s">
         <v>40</v>
@@ -2567,13 +1724,13 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B16" t="s">
         <v>42</v>
       </c>
       <c r="C16" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D16">
         <v>8</v>
@@ -2587,13 +1744,13 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B17" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C17" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D17">
         <v>8</v>
@@ -2607,13 +1764,13 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B18" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C18" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D18">
         <v>8</v>
@@ -2627,13 +1784,13 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B19" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C19" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D19">
         <v>8</v>
@@ -2647,13 +1804,13 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>227</v>
+      </c>
+      <c r="B20" t="s">
+        <v>228</v>
+      </c>
+      <c r="C20" t="s">
         <v>229</v>
-      </c>
-      <c r="B20" t="s">
-        <v>230</v>
-      </c>
-      <c r="C20" t="s">
-        <v>231</v>
       </c>
       <c r="D20">
         <v>8</v>
@@ -2667,10 +1824,10 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B21" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C21" t="s">
         <v>6</v>
@@ -2687,10 +1844,10 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B22" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C22" t="s">
         <v>6</v>
@@ -2707,10 +1864,10 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B23" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C23" t="s">
         <v>6</v>
@@ -2727,10 +1884,10 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B24" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C24" t="s">
         <v>6</v>
@@ -2747,10 +1904,10 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B25" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C25" t="s">
         <v>6</v>
@@ -2767,10 +1924,10 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B26" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C26" t="s">
         <v>6</v>
@@ -2787,10 +1944,10 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B27" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C27" t="s">
         <v>6</v>
@@ -2807,10 +1964,10 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B28" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C28" t="s">
         <v>6</v>
@@ -2827,10 +1984,10 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B29" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C29" t="s">
         <v>6</v>
@@ -2847,10 +2004,10 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B30" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C30" t="s">
         <v>6</v>
@@ -2867,10 +2024,10 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B31" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C31" t="s">
         <v>6</v>
@@ -2887,10 +2044,10 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B32" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C32" t="s">
         <v>6</v>
@@ -2907,10 +2064,10 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B33" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C33" t="s">
         <v>6</v>
@@ -2927,10 +2084,10 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B34" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C34" t="s">
         <v>6</v>
@@ -2947,10 +2104,10 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B35" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C35" t="s">
         <v>6</v>
@@ -2967,10 +2124,10 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B36" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C36" t="s">
         <v>6</v>
@@ -2987,10 +2144,10 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B37" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C37" t="s">
         <v>6</v>
@@ -3007,10 +2164,10 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B38" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C38" t="s">
         <v>6</v>
@@ -3027,10 +2184,10 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B39" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C39" t="s">
         <v>6</v>
@@ -3047,10 +2204,10 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B40" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C40" t="s">
         <v>6</v>
@@ -3067,10 +2224,10 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B41" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C41" t="s">
         <v>6</v>
@@ -3087,10 +2244,10 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B42" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C42" t="s">
         <v>6</v>
@@ -3107,10 +2264,10 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B43" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C43" t="s">
         <v>6</v>
@@ -3127,10 +2284,10 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B44" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C44" t="s">
         <v>6</v>
@@ -3151,11 +2308,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62F8966C-0492-4738-84AA-AA5E0C7A41BB}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
@@ -3191,7 +2348,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -3211,7 +2368,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
@@ -3231,7 +2388,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -3251,7 +2408,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
@@ -3271,7 +2428,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
@@ -3291,7 +2448,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
@@ -3311,7 +2468,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
@@ -3331,7 +2488,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B9" t="s">
         <v>8</v>
@@ -3351,13 +2508,13 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B10" t="s">
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D10">
         <v>10</v>
@@ -3371,7 +2528,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B11" t="s">
         <v>8</v>
@@ -3391,10 +2548,10 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B12" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C12" t="s">
         <v>37</v>
@@ -3411,10 +2568,10 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B13" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C13" t="s">
         <v>10</v>
@@ -3436,154 +2593,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{078A4859-9E32-4DA3-ACFF-EC0D5B5C36FA}">
-  <dimension ref="A1:F12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="22.42578125" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" customWidth="1"/>
-    <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>88</v>
-      </c>
-      <c r="F1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" t="s">
-        <v>170</v>
-      </c>
-      <c r="C2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" t="s">
-        <v>171</v>
-      </c>
-      <c r="C3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4">
-        <v>8</v>
-      </c>
-      <c r="E4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5">
-        <v>16</v>
-      </c>
-      <c r="E5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" t="s">
-        <v>172</v>
-      </c>
-      <c r="C6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6">
-        <v>16</v>
-      </c>
-      <c r="E6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F11" s="1"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F12" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D5E5B8F-5BB7-4168-B07F-5847C1B5455F}">
   <dimension ref="A1:F5"/>
   <sheetViews>
@@ -3629,7 +2638,7 @@
         <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D2">
         <v>8</v>
@@ -3643,7 +2652,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B3" t="s">
         <v>30</v>
@@ -3663,13 +2672,13 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B4" t="s">
         <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D4">
         <v>8</v>
@@ -3683,7 +2692,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
@@ -3706,7 +2715,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDACA481-2925-4EA7-BD1F-BDE6CBFB0E5A}">
   <dimension ref="A1:F16"/>
   <sheetViews>
@@ -3746,7 +2755,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B2" t="s">
         <v>18</v>
@@ -3766,7 +2775,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B3" t="s">
         <v>18</v>
@@ -3786,7 +2795,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B4" t="s">
         <v>18</v>
@@ -3806,7 +2815,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B5" t="s">
         <v>18</v>
@@ -3826,10 +2835,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C6" t="s">
         <v>37</v>
@@ -3846,10 +2855,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C7" t="s">
         <v>37</v>
@@ -3866,10 +2875,10 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C8" t="s">
         <v>37</v>
@@ -3886,10 +2895,10 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C9" t="s">
         <v>37</v>
@@ -3906,10 +2915,10 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C10" t="s">
         <v>37</v>
@@ -3926,10 +2935,10 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C11" t="s">
         <v>37</v>
@@ -3946,10 +2955,10 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C12" t="s">
         <v>37</v>
@@ -3966,10 +2975,10 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C13" t="s">
         <v>37</v>
@@ -3986,10 +2995,10 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C14" t="s">
         <v>37</v>
@@ -4006,10 +3015,10 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B15" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C15" t="s">
         <v>37</v>
@@ -4026,10 +3035,10 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>105</v>
+      </c>
+      <c r="B16" t="s">
         <v>106</v>
-      </c>
-      <c r="B16" t="s">
-        <v>107</v>
       </c>
       <c r="C16" t="s">
         <v>37</v>
@@ -4050,7 +3059,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA3DCDAD-A104-45B0-9B4C-29AE8EC77D31}">
   <dimension ref="A1:F4"/>
   <sheetViews>
@@ -4089,10 +3098,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>10</v>
@@ -4109,13 +3118,13 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D3">
         <v>8</v>
@@ -4129,13 +3138,13 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D4">
         <v>8</v>
@@ -4152,7 +3161,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F712FA06-0E6E-4AB1-8B1E-2EE3C8FE3D18}">
   <dimension ref="A1:F35"/>
   <sheetViews>
@@ -4191,13 +3200,13 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -4211,13 +3220,13 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -4231,13 +3240,13 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -4251,13 +3260,13 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -4271,13 +3280,13 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D6">
         <v>4</v>
@@ -4291,13 +3300,13 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D7">
         <v>2</v>
@@ -4311,13 +3320,13 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D8">
         <v>2</v>
@@ -4331,13 +3340,13 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -4351,13 +3360,13 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B10" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C10" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -4371,13 +3380,13 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B11" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C11" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D11">
         <v>3</v>
@@ -4391,13 +3400,13 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B12" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D12">
         <v>4</v>
@@ -4411,13 +3420,13 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B13" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C13" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D13">
         <v>2</v>
@@ -4431,13 +3440,13 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B14" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C14" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -4451,13 +3460,13 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B15" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C15" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D15">
         <v>2</v>
@@ -4471,10 +3480,10 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C16" t="s">
         <v>38</v>
@@ -4491,10 +3500,10 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B17" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C17" t="s">
         <v>38</v>
@@ -4511,10 +3520,10 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B18" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C18" t="s">
         <v>38</v>
@@ -4531,10 +3540,10 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B19" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C19" t="s">
         <v>38</v>
@@ -4551,10 +3560,10 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B20" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C20" t="s">
         <v>38</v>
@@ -4571,10 +3580,10 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B21" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C21" t="s">
         <v>38</v>
@@ -4591,13 +3600,13 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B22" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C22" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D22">
         <v>4</v>
@@ -4611,13 +3620,13 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B23" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C23" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D23">
         <v>1</v>
@@ -4631,13 +3640,13 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B24" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C24" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D24">
         <v>1</v>
@@ -4651,13 +3660,13 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B25" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C25" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D25">
         <v>1</v>
@@ -4671,13 +3680,13 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B26" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C26" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D26">
         <v>1</v>
@@ -4691,13 +3700,13 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B27" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C27" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D27">
         <v>1</v>
@@ -4711,13 +3720,13 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B28" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C28" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D28">
         <v>1</v>
@@ -4731,13 +3740,13 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B29" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C29" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D29">
         <v>4</v>
@@ -4751,10 +3760,10 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B30" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C30" t="s">
         <v>38</v>
@@ -4771,10 +3780,10 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B31" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C31" t="s">
         <v>38</v>
@@ -4791,10 +3800,10 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B32" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C32" t="s">
         <v>38</v>
@@ -4811,7 +3820,7 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B33" t="s">
         <v>7</v>
@@ -4831,10 +3840,10 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B34" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C34" t="s">
         <v>38</v>
@@ -4851,13 +3860,13 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B35" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C35" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D35">
         <v>8</v>
@@ -4875,7 +3884,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AF12F6B-39D7-464E-AFAC-DA98604DB1A5}">
   <dimension ref="A1:F23"/>
   <sheetViews>
@@ -5095,7 +4104,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B11" t="s">
         <v>34</v>
@@ -5158,7 +4167,7 @@
         <v>39</v>
       </c>
       <c r="B14" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C14" t="s">
         <v>10</v>
@@ -5175,7 +4184,7 @@
     </row>
     <row r="15" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B15" t="s">
         <v>4</v>
@@ -5195,7 +4204,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B16" t="s">
         <v>4</v>
@@ -5215,7 +4224,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B17" t="s">
         <v>33</v>
@@ -5235,7 +4244,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B18" t="s">
         <v>33</v>
@@ -5255,7 +4264,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B19" t="s">
         <v>33</v>
@@ -5275,7 +4284,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B20" t="s">
         <v>33</v>
@@ -5295,7 +4304,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B21" t="s">
         <v>33</v>
@@ -5315,7 +4324,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B22" t="s">
         <v>33</v>
@@ -5335,7 +4344,7 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B23" t="s">
         <v>33</v>
@@ -5351,6 +4360,769 @@
       </c>
       <c r="F23">
         <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C9C2D46-1736-43E0-82AF-3E209A55AC59}">
+  <dimension ref="A1:F37"/>
+  <sheetViews>
+    <sheetView topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.42578125" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2">
+        <v>16</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D3">
+        <v>16</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D4">
+        <v>16</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5">
+        <v>16</v>
+      </c>
+      <c r="E5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6">
+        <v>16</v>
+      </c>
+      <c r="E6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7">
+        <v>16</v>
+      </c>
+      <c r="E7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8">
+        <v>16</v>
+      </c>
+      <c r="E8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9">
+        <v>16</v>
+      </c>
+      <c r="E9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10">
+        <v>16</v>
+      </c>
+      <c r="E10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11">
+        <v>16</v>
+      </c>
+      <c r="E11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" t="s">
+        <v>65</v>
+      </c>
+      <c r="C12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12">
+        <v>16</v>
+      </c>
+      <c r="E12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" t="s">
+        <v>66</v>
+      </c>
+      <c r="C13" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13">
+        <v>16</v>
+      </c>
+      <c r="E13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" t="s">
+        <v>67</v>
+      </c>
+      <c r="C14" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14">
+        <v>16</v>
+      </c>
+      <c r="E14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" t="s">
+        <v>68</v>
+      </c>
+      <c r="C15" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15">
+        <v>16</v>
+      </c>
+      <c r="E15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>54</v>
+      </c>
+      <c r="B16" t="s">
+        <v>69</v>
+      </c>
+      <c r="C16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16">
+        <v>16</v>
+      </c>
+      <c r="E16" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>55</v>
+      </c>
+      <c r="B17" t="s">
+        <v>70</v>
+      </c>
+      <c r="C17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17">
+        <v>16</v>
+      </c>
+      <c r="E17" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>73</v>
+      </c>
+      <c r="B18" t="s">
+        <v>58</v>
+      </c>
+      <c r="C18" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>13</v>
+      </c>
+      <c r="F18">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>74</v>
+      </c>
+      <c r="B19" t="s">
+        <v>58</v>
+      </c>
+      <c r="C19" t="s">
+        <v>37</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>12</v>
+      </c>
+      <c r="F19">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>75</v>
+      </c>
+      <c r="B20" t="s">
+        <v>58</v>
+      </c>
+      <c r="C20" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>11</v>
+      </c>
+      <c r="F20">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>76</v>
+      </c>
+      <c r="B21" t="s">
+        <v>58</v>
+      </c>
+      <c r="C21" t="s">
+        <v>37</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <v>10</v>
+      </c>
+      <c r="F21">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>77</v>
+      </c>
+      <c r="B22" t="s">
+        <v>58</v>
+      </c>
+      <c r="C22" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>9</v>
+      </c>
+      <c r="F22">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>78</v>
+      </c>
+      <c r="B23" t="s">
+        <v>58</v>
+      </c>
+      <c r="C23" t="s">
+        <v>37</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>8</v>
+      </c>
+      <c r="F23">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>79</v>
+      </c>
+      <c r="B24" t="s">
+        <v>58</v>
+      </c>
+      <c r="C24" t="s">
+        <v>37</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>7</v>
+      </c>
+      <c r="F24">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>80</v>
+      </c>
+      <c r="B25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C25" t="s">
+        <v>37</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <v>6</v>
+      </c>
+      <c r="F25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>81</v>
+      </c>
+      <c r="B26" t="s">
+        <v>58</v>
+      </c>
+      <c r="C26" t="s">
+        <v>37</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <v>5</v>
+      </c>
+      <c r="F26">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>82</v>
+      </c>
+      <c r="B27" t="s">
+        <v>58</v>
+      </c>
+      <c r="C27" t="s">
+        <v>37</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>4</v>
+      </c>
+      <c r="F27">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>83</v>
+      </c>
+      <c r="B28" t="s">
+        <v>58</v>
+      </c>
+      <c r="C28" t="s">
+        <v>37</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28">
+        <v>3</v>
+      </c>
+      <c r="F28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>84</v>
+      </c>
+      <c r="B29" t="s">
+        <v>58</v>
+      </c>
+      <c r="C29" t="s">
+        <v>37</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <v>2</v>
+      </c>
+      <c r="F29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>85</v>
+      </c>
+      <c r="B30" t="s">
+        <v>58</v>
+      </c>
+      <c r="C30" t="s">
+        <v>37</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+      <c r="F30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>86</v>
+      </c>
+      <c r="B31" t="s">
+        <v>58</v>
+      </c>
+      <c r="C31" t="s">
+        <v>37</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>108</v>
+      </c>
+      <c r="B32" t="s">
+        <v>106</v>
+      </c>
+      <c r="C32" t="s">
+        <v>10</v>
+      </c>
+      <c r="D32">
+        <v>32</v>
+      </c>
+      <c r="E32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F32" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>107</v>
+      </c>
+      <c r="B33" t="s">
+        <v>30</v>
+      </c>
+      <c r="C33" t="s">
+        <v>10</v>
+      </c>
+      <c r="D33">
+        <v>32</v>
+      </c>
+      <c r="E33" t="s">
+        <v>9</v>
+      </c>
+      <c r="F33" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>109</v>
+      </c>
+      <c r="B34" t="s">
+        <v>40</v>
+      </c>
+      <c r="C34" t="s">
+        <v>10</v>
+      </c>
+      <c r="D34">
+        <v>32</v>
+      </c>
+      <c r="E34" t="s">
+        <v>9</v>
+      </c>
+      <c r="F34" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>110</v>
+      </c>
+      <c r="B35" t="s">
+        <v>42</v>
+      </c>
+      <c r="C35" t="s">
+        <v>10</v>
+      </c>
+      <c r="D35">
+        <v>32</v>
+      </c>
+      <c r="E35" t="s">
+        <v>9</v>
+      </c>
+      <c r="F35" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>112</v>
+      </c>
+      <c r="B36" t="s">
+        <v>4</v>
+      </c>
+      <c r="C36" t="s">
+        <v>37</v>
+      </c>
+      <c r="D36">
+        <v>1</v>
+      </c>
+      <c r="E36">
+        <v>8</v>
+      </c>
+      <c r="F36">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>111</v>
+      </c>
+      <c r="B37" t="s">
+        <v>4</v>
+      </c>
+      <c r="C37" t="s">
+        <v>37</v>
+      </c>
+      <c r="D37">
+        <v>1</v>
+      </c>
+      <c r="E37">
+        <v>9</v>
+      </c>
+      <c r="F37">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -5360,21 +5132,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B40B7BE3-9A42-42BA-88D6-9D009061040B}">
-  <dimension ref="A1:F4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{427C2A19-8BF7-4B8D-9492-08A4DEB2EF8C}">
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.42578125" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -5394,66 +5159,6 @@
       </c>
       <c r="F1" t="s">
         <v>89</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2">
-        <v>32</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3">
-        <v>32</v>
-      </c>
-      <c r="E3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>90</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>4</v>
-      </c>
-      <c r="F4">
-        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -5462,21 +5167,14 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE81132C-CE5C-48CD-A64A-B3A385985B9A}">
-  <dimension ref="A1:F4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9F9F601-34D5-480B-81CE-67CE1CDB2EB8}">
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.42578125" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" customWidth="1"/>
-    <col min="6" max="6" width="14" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -5496,66 +5194,6 @@
       </c>
       <c r="F1" t="s">
         <v>89</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2">
-        <v>32</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3">
-        <v>32</v>
-      </c>
-      <c r="E3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>90</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>5</v>
-      </c>
-      <c r="F4">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>